<commit_message>
update tài liêu đã chỉnh sửa nhờ anh vũ review
</commit_message>
<xml_diff>
--- a/2015/201512/10_DOCUMENT/13_DETAIL_DESIGN/Bao cao khach hang moi theo nhan vien/CRMFXXX1_Bao cao KH moi theo NV.xlsx
+++ b/2015/201512/10_DOCUMENT/13_DETAIL_DESIGN/Bao cao khach hang moi theo nhan vien/CRMFXXX1_Bao cao KH moi theo NV.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="15480" windowHeight="9990" tabRatio="836" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="15480" windowHeight="9990" tabRatio="836" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Coverpage" sheetId="20" r:id="rId1"/>
@@ -18,8 +18,8 @@
     <sheet name="Item Screen" sheetId="15" r:id="rId4"/>
     <sheet name="Input Check" sheetId="16" r:id="rId5"/>
     <sheet name="Data Definition" sheetId="18" r:id="rId6"/>
-    <sheet name="Data Input" sheetId="13" r:id="rId7"/>
-    <sheet name="Form Func Spec" sheetId="14" r:id="rId8"/>
+    <sheet name="Form Func Spec" sheetId="14" r:id="rId7"/>
+    <sheet name="Data Input" sheetId="13" r:id="rId8"/>
     <sheet name="Func Spec" sheetId="17" r:id="rId9"/>
     <sheet name="Help" sheetId="6" r:id="rId10"/>
     <sheet name="Code Standar" sheetId="19" r:id="rId11"/>
@@ -44,8 +44,8 @@
     <definedName name="OLE_LINK1" localSheetId="10">'Code Standar'!$B$2</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Coverpage!$A$1:$J$31</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="5">'Data Definition'!$A$1:$P$58</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="6">'Data Input'!$A$1:$R$94</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="7">'Form Func Spec'!$A$1:$J$52</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="7">'Data Input'!$A$1:$R$94</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="6">'Form Func Spec'!$A$1:$J$52</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="8">'Func Spec'!$A$1:$J$32</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="9">Help!$A$1:$K$62</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="4">'Input Check'!$A$1:$I$54</definedName>
@@ -999,170 +999,6 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>vinhphong</author>
-    <author>Le Thi Thu Hien</author>
-  </authors>
-  <commentList>
-    <comment ref="P1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Người cập nhật tài liệu</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="P2" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Ngày tạo tài liệu</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G4" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Loại SQL thực thi:
-- Select = S
-- Insert = I
-- Delete = D
-- Update = U</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H4" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Hinh thức SQL:
-- ID: sử dụng cho trường hợp SQL Script đã được lưu thành file
-- SQL Script: sử dụng trực tiếp SQL để thực thi</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I4" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>ID của:
-- SQL Script
-- Store
-- Function
-- Trigger
-Câu đổ nguồn chuẩn</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J4" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">SQL sử dụng để thực thi trực tiếp
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="N4" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Tên của Parameter
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="O4" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Giá trị truyền vào Parameter
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="Q4" authorId="1" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Sự kiện</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>vinhphong</author>
     <author>binhminh</author>
   </authors>
   <commentList>
@@ -1382,6 +1218,170 @@
 </comments>
 </file>
 
+<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>vinhphong</author>
+    <author>Le Thi Thu Hien</author>
+  </authors>
+  <commentList>
+    <comment ref="P1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Người cập nhật tài liệu</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ngày tạo tài liệu</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G4" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Loại SQL thực thi:
+- Select = S
+- Insert = I
+- Delete = D
+- Update = U</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H4" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Hinh thức SQL:
+- ID: sử dụng cho trường hợp SQL Script đã được lưu thành file
+- SQL Script: sử dụng trực tiếp SQL để thực thi</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I4" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>ID của:
+- SQL Script
+- Store
+- Function
+- Trigger
+Câu đổ nguồn chuẩn</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J4" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">SQL sử dụng để thực thi trực tiếp
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N4" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Tên của Parameter
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O4" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Giá trị truyền vào Parameter
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q4" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sự kiện</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
@@ -1551,7 +1551,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="239">
   <si>
     <t>Detail Design</t>
   </si>
@@ -2160,9 +2160,6 @@
     <t>In</t>
   </si>
   <si>
-    <t>CheckBox</t>
-  </si>
-  <si>
     <t>Button</t>
   </si>
   <si>
@@ -2197,9 +2194,6 @@
   </si>
   <si>
     <t>Boolean</t>
-  </si>
-  <si>
-    <t>Truyền tham số @DivisionID để gọi load báo cáo khi in</t>
   </si>
   <si>
     <t>Click vào Button In</t>
@@ -2254,19 +2248,7 @@
     <t>DropDownCheckList</t>
   </si>
   <si>
-    <t>Xem trước</t>
-  </si>
-  <si>
-    <t>BttView</t>
-  </si>
-  <si>
     <t>AccountID</t>
-  </si>
-  <si>
-    <t>Click vào Button Xem trước</t>
-  </si>
-  <si>
-    <t>Truyền tham số @DivisionID để gọi load màn hình báo cáo trước khi in</t>
   </si>
   <si>
     <t>Đổ nguồn combobox Khách hàng</t>
@@ -2293,36 +2275,18 @@
 Order By EmployeeID</t>
   </si>
   <si>
-    <t>Checkbox1</t>
-  </si>
-  <si>
-    <t>Checkbox2</t>
-  </si>
-  <si>
     <t>EmployeeID</t>
   </si>
   <si>
-    <t>Thực thi @SQL0003 khi CheckBox1 = 1</t>
-  </si>
-  <si>
-    <t>Thực thi @SQL0004 khi CheckBox2 = 1</t>
-  </si>
-  <si>
     <t>Thực thi @SQL0001 , @SQL0002, @SQL0003 và @SQL0004 đổ nguồn cho combo/Dropdownchecklist</t>
   </si>
   <si>
-    <t>Click vào BttnView thực thi @SQL0005 Load màn hình view trước khi In</t>
-  </si>
-  <si>
     <t>Load màn hình Báo cáo để xem trước khi in</t>
   </si>
   <si>
     <t>@SQL0005</t>
   </si>
   <si>
-    <t>Click BttnView</t>
-  </si>
-  <si>
     <t>Click CheckBox1</t>
   </si>
   <si>
@@ -2332,20 +2296,54 @@
     <t>thực thi @SQL0005 để load báo cáo khách hàng theo nhân viên xem trước khi in</t>
   </si>
   <si>
-    <t>@DivisionID @DivisionIDList  @FromDate @ToDate   @IsDate  
-@CheckBox1
-@FromAccountID @ToAccountID 
-@CheckBox2 @FromEmployeeID@ToEmployeeID @UserID
-@PageNumber
-@PageSize</t>
-  </si>
-  <si>
-    <t>Biến môi trường @@DivisionIDList  @@FromDate @@ToDate   @@IsDate 
-0,1 
-@@FromAccountID @@ToAccountID
-0,1 @@FromEmployeeID @@ToEmployeeID Biến môi trường
-@@PageNumber
-@@PageSize</t>
+    <t>FromAccountID</t>
+  </si>
+  <si>
+    <t>Từ Khách hàng</t>
+  </si>
+  <si>
+    <t>Đến Khách hàng</t>
+  </si>
+  <si>
+    <t>Từ Nhân viên</t>
+  </si>
+  <si>
+    <t>Đến Nhân viên</t>
+  </si>
+  <si>
+    <t>ToAccountID</t>
+  </si>
+  <si>
+    <t>FromEmployeeID</t>
+  </si>
+  <si>
+    <t>ToEmployeeID</t>
+  </si>
+  <si>
+    <t>Nếu được Check vào thì đổ Combobox</t>
+  </si>
+  <si>
+    <t>Báo cáo -&gt; Báo cáo Thống kê 
+-&gt; Click vào Báo cáo KH mới theo nhân viên 
+-&gt; Hiển thị màn hình Báo cáo khách hàng mới theo nhân viên</t>
+  </si>
+  <si>
+    <t>Đóng</t>
+  </si>
+  <si>
+    <t>BttnClose</t>
+  </si>
+  <si>
+    <t>Đóng màn hình báo cáo</t>
+  </si>
+  <si>
+    <t>Truyền tham số @DivisionID để gọi tab màn hình báo cáo khi in</t>
+  </si>
+  <si>
+    <t>Đổ nguồn Combobox Khách hàng</t>
+  </si>
+  <si>
+    <t>Đổ nguồn Combobox Nhân viên</t>
   </si>
   <si>
     <t xml:space="preserve">EXEC CRMP10104(
@@ -2354,10 +2352,8 @@
   @FromDate         DATETIME,
   @ToDate           DATETIME,
   @IsDate           TINYINT,
-@CheckBox1 TINYINT,
 @FromAccountID       Varchar(50),
   @ToAccountID         Varchar(50),
-@CheckBox2 TINYINT,
   @FromEmployeeID           Varchar(50),
   @ToEmployeeID           Varchar(50),
   @UserID  VARCHAR(50),
@@ -2366,31 +2362,36 @@
 </t>
   </si>
   <si>
-    <t>FromAccountID</t>
-  </si>
-  <si>
-    <t>Từ Khách hàng</t>
-  </si>
-  <si>
-    <t>Đến Khách hàng</t>
-  </si>
-  <si>
-    <t>Từ Nhân viên</t>
-  </si>
-  <si>
-    <t>Đến Nhân viên</t>
-  </si>
-  <si>
-    <t>ToAccountID</t>
-  </si>
-  <si>
-    <t>FromEmployeeID</t>
-  </si>
-  <si>
-    <t>ToEmployeeID</t>
-  </si>
-  <si>
-    <t>Nếu được Check vào thì đổ Combobox</t>
+    <t>@DivisionID @DivisionIDList  @FromDate @ToDate   @IsDate  
+@FromAccountID @ToAccountID 
+FromEmployeeID@ToEmployeeID @UserID
+@PageNumber
+@PageSize</t>
+  </si>
+  <si>
+    <t>Biến môi trường @@DivisionIDList  @@FromDate @@ToDate   @@IsDate 
+@@FromAccountID @@ToAccountID
+@@FromEmployeeID @@ToEmployeeID Biến môi trường
+@@PageNumber
+@@PageSize</t>
+  </si>
+  <si>
+    <t>@ReportID</t>
+  </si>
+  <si>
+    <t>Click vào Báo cáo Khách hàng mới theo nhân viên</t>
+  </si>
+  <si>
+    <t>Click BttnPrint</t>
+  </si>
+  <si>
+    <t>Click vào BttnPrint thực thi @SQL0005 Load màn hình view trước khi In</t>
+  </si>
+  <si>
+    <t>CRMF3010</t>
+  </si>
+  <si>
+    <t>Nhận tham số @ReportID từ màn hình Báo cáo biểu đồ CRMT3002 để mởi màn hình CRMF3010</t>
   </si>
 </sst>
 </file>
@@ -3542,20 +3543,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>3285759</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>771525</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="3" name="Picture 2"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -3575,8 +3576,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="104775" y="723900"/>
-          <a:ext cx="10058034" cy="4933950"/>
+          <a:off x="2381250" y="1304925"/>
+          <a:ext cx="4419600" cy="3257550"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5498,7 +5499,7 @@
   <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19:J19"/>
+      <selection activeCell="E13" sqref="E13:J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1"/>
@@ -5528,7 +5529,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="36" t="s">
-        <v>160</v>
+        <v>237</v>
       </c>
       <c r="G1" s="31" t="s">
         <v>5</v>
@@ -6274,7 +6275,7 @@
   <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12:J43"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1"/>
@@ -6286,7 +6287,7 @@
     <col min="5" max="5" width="12.85546875" style="22" customWidth="1"/>
     <col min="6" max="6" width="31.7109375" style="22" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" style="22" customWidth="1"/>
-    <col min="8" max="8" width="51.85546875" style="22" customWidth="1"/>
+    <col min="8" max="8" width="29" style="22" customWidth="1"/>
     <col min="9" max="9" width="13.140625" style="22" customWidth="1"/>
     <col min="10" max="10" width="12.7109375" style="22" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="22"/>
@@ -6309,7 +6310,7 @@
       </c>
       <c r="F1" s="36" t="str">
         <f>'Update History'!F1</f>
-        <v>CRMFXXX1</v>
+        <v>CRMF3010</v>
       </c>
       <c r="G1" s="31" t="s">
         <v>5</v>
@@ -6382,7 +6383,7 @@
       <c r="G5" s="43"/>
       <c r="H5" s="44"/>
       <c r="I5" s="179" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J5" s="180"/>
     </row>
@@ -6469,7 +6470,9 @@
       <c r="F12" s="43"/>
       <c r="G12" s="43"/>
       <c r="H12" s="45"/>
-      <c r="I12" s="173"/>
+      <c r="I12" s="173" t="s">
+        <v>223</v>
+      </c>
       <c r="J12" s="174"/>
     </row>
     <row r="13" spans="1:10" ht="12" customHeight="1">
@@ -6870,13 +6873,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O61"/>
+  <dimension ref="A1:O58"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="124" zoomScaleNormal="100" zoomScaleSheetLayoutView="124" workbookViewId="0">
-      <pane xSplit="6" ySplit="4" topLeftCell="G5" activePane="bottomRight" state="frozen"/>
+    <sheetView view="pageBreakPreview" zoomScale="124" zoomScaleNormal="100" zoomScaleSheetLayoutView="124" workbookViewId="0">
+      <pane xSplit="6" ySplit="4" topLeftCell="N5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="H15" sqref="H15"/>
+      <selection pane="bottomRight" activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1"/>
@@ -7035,7 +7038,7 @@
       </c>
       <c r="E5" s="83" t="str">
         <f>'Update History'!F1</f>
-        <v>CRMFXXX1</v>
+        <v>CRMF3010</v>
       </c>
       <c r="F5" s="69"/>
       <c r="G5" s="40" t="s">
@@ -7062,14 +7065,14 @@
       </c>
       <c r="D6" s="59"/>
       <c r="E6" s="88" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F6" s="88"/>
       <c r="G6" s="40" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H6" s="40" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I6" s="62"/>
       <c r="J6" s="62"/>
@@ -7093,16 +7096,16 @@
         <v>166</v>
       </c>
       <c r="E7" s="88" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F7" s="127" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G7" s="40" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H7" s="40" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I7" s="62"/>
       <c r="J7" s="62"/>
@@ -7128,16 +7131,16 @@
         <v>167</v>
       </c>
       <c r="E8" s="88" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F8" s="127" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G8" s="40" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H8" s="40" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I8" s="62"/>
       <c r="J8" s="62"/>
@@ -7161,14 +7164,14 @@
       </c>
       <c r="D9" s="59"/>
       <c r="E9" s="127" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F9" s="127"/>
       <c r="G9" s="40" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H9" s="40" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I9" s="62"/>
       <c r="J9" s="62"/>
@@ -7192,16 +7195,16 @@
         <v>168</v>
       </c>
       <c r="E10" s="88" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F10" s="127" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G10" s="40" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="H10" s="40" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I10" s="62"/>
       <c r="J10" s="62"/>
@@ -7227,16 +7230,16 @@
         <v>169</v>
       </c>
       <c r="E11" s="88" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F11" s="127" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G11" s="40" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="H11" s="40" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I11" s="62">
         <v>50</v>
@@ -7258,24 +7261,34 @@
       <c r="C12" s="33">
         <v>8</v>
       </c>
-      <c r="D12" s="59"/>
+      <c r="D12" s="59" t="s">
+        <v>215</v>
+      </c>
       <c r="E12" s="133" t="s">
-        <v>213</v>
-      </c>
-      <c r="F12" s="133"/>
+        <v>214</v>
+      </c>
+      <c r="F12" s="133" t="s">
+        <v>200</v>
+      </c>
       <c r="G12" s="40" t="s">
-        <v>171</v>
-      </c>
-      <c r="H12" s="40"/>
-      <c r="I12" s="62"/>
+        <v>173</v>
+      </c>
+      <c r="H12" s="40" t="s">
+        <v>180</v>
+      </c>
+      <c r="I12" s="62">
+        <v>50</v>
+      </c>
       <c r="J12" s="62"/>
-      <c r="K12" s="40"/>
+      <c r="K12" s="40" t="s">
+        <v>150</v>
+      </c>
       <c r="L12" s="133"/>
       <c r="M12" s="133"/>
-      <c r="N12" s="133">
-        <v>0</v>
-      </c>
-      <c r="O12" s="133"/>
+      <c r="N12" s="133"/>
+      <c r="O12" s="133" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="13" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A13" s="33">
@@ -7288,33 +7301,29 @@
         <v>9</v>
       </c>
       <c r="D13" s="59" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
       <c r="E13" s="133" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="F13" s="133" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="G13" s="40" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H13" s="40" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I13" s="62">
         <v>50</v>
       </c>
       <c r="J13" s="62"/>
-      <c r="K13" s="40" t="s">
-        <v>150</v>
-      </c>
+      <c r="K13" s="40"/>
       <c r="L13" s="133"/>
       <c r="M13" s="133"/>
       <c r="N13" s="133"/>
-      <c r="O13" s="133" t="s">
-        <v>237</v>
-      </c>
+      <c r="O13" s="133"/>
     </row>
     <row r="14" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A14" s="33">
@@ -7327,29 +7336,33 @@
         <v>10</v>
       </c>
       <c r="D14" s="59" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="E14" s="133" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="F14" s="133" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="G14" s="40" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H14" s="40" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I14" s="62">
         <v>50</v>
       </c>
       <c r="J14" s="62"/>
-      <c r="K14" s="40"/>
+      <c r="K14" s="40" t="s">
+        <v>150</v>
+      </c>
       <c r="L14" s="133"/>
       <c r="M14" s="133"/>
       <c r="N14" s="133"/>
-      <c r="O14" s="133"/>
+      <c r="O14" s="133" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="15" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A15" s="33">
@@ -7361,26 +7374,32 @@
       <c r="C15" s="33">
         <v>11</v>
       </c>
-      <c r="D15" s="59"/>
+      <c r="D15" s="59" t="s">
+        <v>218</v>
+      </c>
       <c r="E15" s="133" t="s">
-        <v>214</v>
-      </c>
-      <c r="F15" s="133"/>
+        <v>221</v>
+      </c>
+      <c r="F15" s="133" t="s">
+        <v>207</v>
+      </c>
       <c r="G15" s="40" t="s">
-        <v>171</v>
-      </c>
-      <c r="H15" s="40"/>
-      <c r="I15" s="62"/>
+        <v>173</v>
+      </c>
+      <c r="H15" s="40" t="s">
+        <v>180</v>
+      </c>
+      <c r="I15" s="62">
+        <v>50</v>
+      </c>
       <c r="J15" s="62"/>
       <c r="K15" s="40"/>
       <c r="L15" s="133"/>
       <c r="M15" s="133"/>
-      <c r="N15" s="133">
-        <v>0</v>
-      </c>
+      <c r="N15" s="133"/>
       <c r="O15" s="133"/>
     </row>
-    <row r="16" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
+    <row r="16" spans="1:15" s="34" customFormat="1" ht="11.25">
       <c r="A16" s="33">
         <v>12</v>
       </c>
@@ -7391,33 +7410,23 @@
         <v>12</v>
       </c>
       <c r="D16" s="59" t="s">
-        <v>232</v>
-      </c>
-      <c r="E16" s="133" t="s">
-        <v>235</v>
-      </c>
-      <c r="F16" s="133" t="s">
-        <v>215</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="E16" s="88" t="s">
+        <v>179</v>
+      </c>
+      <c r="F16" s="88"/>
       <c r="G16" s="40" t="s">
-        <v>174</v>
-      </c>
-      <c r="H16" s="40" t="s">
-        <v>181</v>
-      </c>
-      <c r="I16" s="62">
-        <v>50</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="H16" s="40"/>
+      <c r="I16" s="62"/>
       <c r="J16" s="62"/>
-      <c r="K16" s="40" t="s">
-        <v>150</v>
-      </c>
-      <c r="L16" s="133"/>
-      <c r="M16" s="133"/>
-      <c r="N16" s="133"/>
-      <c r="O16" s="133" t="s">
-        <v>237</v>
-      </c>
+      <c r="K16" s="40"/>
+      <c r="L16" s="90"/>
+      <c r="M16" s="69"/>
+      <c r="N16" s="69"/>
+      <c r="O16" s="88"/>
     </row>
     <row r="17" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A17" s="33">
@@ -7430,84 +7439,60 @@
         <v>13</v>
       </c>
       <c r="D17" s="59" t="s">
-        <v>233</v>
-      </c>
-      <c r="E17" s="133" t="s">
-        <v>236</v>
-      </c>
-      <c r="F17" s="133" t="s">
-        <v>215</v>
-      </c>
+        <v>224</v>
+      </c>
+      <c r="E17" s="88" t="s">
+        <v>225</v>
+      </c>
+      <c r="F17" s="84"/>
       <c r="G17" s="40" t="s">
-        <v>174</v>
-      </c>
-      <c r="H17" s="40" t="s">
-        <v>181</v>
-      </c>
-      <c r="I17" s="62">
-        <v>50</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="H17" s="40"/>
+      <c r="I17" s="62"/>
       <c r="J17" s="62"/>
       <c r="K17" s="40"/>
-      <c r="L17" s="133"/>
-      <c r="M17" s="133"/>
-      <c r="N17" s="133"/>
-      <c r="O17" s="133"/>
-    </row>
-    <row r="18" spans="1:15" s="34" customFormat="1" ht="11.25">
+      <c r="L17" s="90"/>
+      <c r="M17" s="69"/>
+      <c r="N17" s="69"/>
+      <c r="O17" s="88" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A18" s="33">
         <v>14</v>
       </c>
-      <c r="B18" s="33" t="s">
-        <v>164</v>
-      </c>
-      <c r="C18" s="33">
-        <v>14</v>
-      </c>
-      <c r="D18" s="59" t="s">
-        <v>202</v>
-      </c>
-      <c r="E18" s="133" t="s">
-        <v>203</v>
-      </c>
-      <c r="F18" s="133"/>
-      <c r="G18" s="40" t="s">
-        <v>172</v>
-      </c>
+      <c r="B18" s="33"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="88"/>
+      <c r="F18" s="88"/>
+      <c r="G18" s="40"/>
       <c r="H18" s="40"/>
       <c r="I18" s="62"/>
       <c r="J18" s="62"/>
       <c r="K18" s="40"/>
-      <c r="L18" s="133"/>
-      <c r="M18" s="133"/>
-      <c r="N18" s="133"/>
-      <c r="O18" s="133"/>
-    </row>
-    <row r="19" spans="1:15" s="34" customFormat="1" ht="11.25">
+      <c r="L18" s="62"/>
+      <c r="M18" s="69"/>
+      <c r="N18" s="69"/>
+      <c r="O18" s="88"/>
+    </row>
+    <row r="19" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A19" s="33">
         <v>15</v>
       </c>
-      <c r="B19" s="33" t="s">
-        <v>164</v>
-      </c>
-      <c r="C19" s="33">
-        <v>15</v>
-      </c>
-      <c r="D19" s="59" t="s">
-        <v>170</v>
-      </c>
-      <c r="E19" s="88" t="s">
-        <v>180</v>
-      </c>
-      <c r="F19" s="88"/>
-      <c r="G19" s="40" t="s">
-        <v>172</v>
-      </c>
+      <c r="B19" s="33"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="59"/>
+      <c r="E19" s="88"/>
+      <c r="F19" s="84"/>
+      <c r="G19" s="40"/>
       <c r="H19" s="40"/>
       <c r="I19" s="62"/>
       <c r="J19" s="62"/>
       <c r="K19" s="40"/>
-      <c r="L19" s="90"/>
+      <c r="L19" s="62"/>
       <c r="M19" s="69"/>
       <c r="N19" s="69"/>
       <c r="O19" s="88"/>
@@ -7520,13 +7505,13 @@
       <c r="C20" s="33"/>
       <c r="D20" s="59"/>
       <c r="E20" s="88"/>
-      <c r="F20" s="84"/>
+      <c r="F20" s="88"/>
       <c r="G20" s="40"/>
       <c r="H20" s="40"/>
       <c r="I20" s="62"/>
       <c r="J20" s="62"/>
       <c r="K20" s="40"/>
-      <c r="L20" s="90"/>
+      <c r="L20" s="62"/>
       <c r="M20" s="69"/>
       <c r="N20" s="69"/>
       <c r="O20" s="88"/>
@@ -7543,54 +7528,54 @@
       <c r="G21" s="40"/>
       <c r="H21" s="40"/>
       <c r="I21" s="62"/>
-      <c r="J21" s="62"/>
+      <c r="J21" s="40"/>
       <c r="K21" s="40"/>
-      <c r="L21" s="62"/>
+      <c r="L21" s="69"/>
       <c r="M21" s="69"/>
       <c r="N21" s="69"/>
       <c r="O21" s="88"/>
     </row>
     <row r="22" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A22" s="33">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B22" s="33"/>
       <c r="C22" s="33"/>
       <c r="D22" s="59"/>
       <c r="E22" s="88"/>
-      <c r="F22" s="84"/>
+      <c r="F22" s="88"/>
       <c r="G22" s="40"/>
       <c r="H22" s="40"/>
-      <c r="I22" s="62"/>
-      <c r="J22" s="62"/>
+      <c r="I22" s="40"/>
+      <c r="J22" s="40"/>
       <c r="K22" s="40"/>
-      <c r="L22" s="62"/>
-      <c r="M22" s="69"/>
+      <c r="L22" s="40"/>
+      <c r="M22" s="40"/>
       <c r="N22" s="69"/>
       <c r="O22" s="88"/>
     </row>
     <row r="23" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A23" s="33">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B23" s="33"/>
       <c r="C23" s="33"/>
       <c r="D23" s="59"/>
       <c r="E23" s="88"/>
-      <c r="F23" s="88"/>
+      <c r="F23" s="84"/>
       <c r="G23" s="40"/>
       <c r="H23" s="40"/>
-      <c r="I23" s="62"/>
-      <c r="J23" s="62"/>
+      <c r="I23" s="40"/>
+      <c r="J23" s="40"/>
       <c r="K23" s="40"/>
-      <c r="L23" s="62"/>
-      <c r="M23" s="69"/>
-      <c r="N23" s="69"/>
+      <c r="L23" s="40"/>
+      <c r="M23" s="40"/>
+      <c r="N23" s="83"/>
       <c r="O23" s="88"/>
     </row>
     <row r="24" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A24" s="33">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B24" s="33"/>
       <c r="C24" s="33"/>
@@ -7599,17 +7584,17 @@
       <c r="F24" s="88"/>
       <c r="G24" s="40"/>
       <c r="H24" s="40"/>
-      <c r="I24" s="62"/>
+      <c r="I24" s="40"/>
       <c r="J24" s="40"/>
       <c r="K24" s="40"/>
-      <c r="L24" s="69"/>
-      <c r="M24" s="69"/>
+      <c r="L24" s="40"/>
+      <c r="M24" s="40"/>
       <c r="N24" s="69"/>
       <c r="O24" s="88"/>
     </row>
     <row r="25" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A25" s="33">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B25" s="33"/>
       <c r="C25" s="33"/>
@@ -7628,13 +7613,13 @@
     </row>
     <row r="26" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A26" s="33">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B26" s="33"/>
       <c r="C26" s="33"/>
       <c r="D26" s="59"/>
       <c r="E26" s="88"/>
-      <c r="F26" s="84"/>
+      <c r="F26" s="88"/>
       <c r="G26" s="40"/>
       <c r="H26" s="40"/>
       <c r="I26" s="40"/>
@@ -7642,12 +7627,12 @@
       <c r="K26" s="40"/>
       <c r="L26" s="40"/>
       <c r="M26" s="40"/>
-      <c r="N26" s="83"/>
+      <c r="N26" s="88"/>
       <c r="O26" s="88"/>
     </row>
     <row r="27" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A27" s="33">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B27" s="33"/>
       <c r="C27" s="33"/>
@@ -7666,89 +7651,89 @@
     </row>
     <row r="28" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A28" s="33">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B28" s="33"/>
       <c r="C28" s="33"/>
       <c r="D28" s="59"/>
-      <c r="E28" s="88"/>
-      <c r="F28" s="88"/>
+      <c r="E28" s="84"/>
+      <c r="F28" s="84"/>
       <c r="G28" s="40"/>
       <c r="H28" s="40"/>
       <c r="I28" s="40"/>
-      <c r="J28" s="40"/>
+      <c r="J28" s="61"/>
       <c r="K28" s="40"/>
-      <c r="L28" s="40"/>
-      <c r="M28" s="40"/>
-      <c r="N28" s="69"/>
-      <c r="O28" s="88"/>
+      <c r="L28" s="61"/>
+      <c r="M28" s="61"/>
+      <c r="N28" s="40"/>
+      <c r="O28" s="32"/>
     </row>
     <row r="29" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A29" s="33">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B29" s="33"/>
       <c r="C29" s="33"/>
       <c r="D29" s="59"/>
       <c r="E29" s="88"/>
-      <c r="F29" s="88"/>
+      <c r="F29" s="83"/>
       <c r="G29" s="40"/>
       <c r="H29" s="40"/>
       <c r="I29" s="40"/>
-      <c r="J29" s="40"/>
+      <c r="J29" s="61"/>
       <c r="K29" s="40"/>
-      <c r="L29" s="40"/>
-      <c r="M29" s="40"/>
-      <c r="N29" s="88"/>
-      <c r="O29" s="88"/>
+      <c r="L29" s="62"/>
+      <c r="M29" s="61"/>
+      <c r="N29" s="61"/>
+      <c r="O29" s="32"/>
     </row>
     <row r="30" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A30" s="33">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B30" s="33"/>
       <c r="C30" s="33"/>
-      <c r="D30" s="59"/>
-      <c r="E30" s="88"/>
-      <c r="F30" s="88"/>
+      <c r="D30" s="87"/>
+      <c r="E30" s="87"/>
+      <c r="F30" s="40"/>
       <c r="G30" s="40"/>
       <c r="H30" s="40"/>
       <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="J30" s="61"/>
       <c r="K30" s="40"/>
-      <c r="L30" s="40"/>
-      <c r="M30" s="40"/>
-      <c r="N30" s="69"/>
-      <c r="O30" s="88"/>
+      <c r="L30" s="62"/>
+      <c r="M30" s="61"/>
+      <c r="N30" s="61"/>
+      <c r="O30" s="32"/>
     </row>
     <row r="31" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A31" s="33">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B31" s="33"/>
       <c r="C31" s="33"/>
-      <c r="D31" s="59"/>
-      <c r="E31" s="84"/>
-      <c r="F31" s="84"/>
+      <c r="D31" s="69"/>
+      <c r="E31" s="69"/>
+      <c r="F31" s="40"/>
       <c r="G31" s="40"/>
       <c r="H31" s="40"/>
       <c r="I31" s="40"/>
       <c r="J31" s="61"/>
       <c r="K31" s="40"/>
-      <c r="L31" s="61"/>
+      <c r="L31" s="62"/>
       <c r="M31" s="61"/>
-      <c r="N31" s="40"/>
+      <c r="N31" s="61"/>
       <c r="O31" s="32"/>
     </row>
     <row r="32" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A32" s="33">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B32" s="33"/>
       <c r="C32" s="33"/>
-      <c r="D32" s="59"/>
-      <c r="E32" s="88"/>
-      <c r="F32" s="83"/>
+      <c r="D32" s="69"/>
+      <c r="E32" s="69"/>
+      <c r="F32" s="40"/>
       <c r="G32" s="40"/>
       <c r="H32" s="40"/>
       <c r="I32" s="40"/>
@@ -7761,12 +7746,12 @@
     </row>
     <row r="33" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A33" s="33">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B33" s="33"/>
       <c r="C33" s="33"/>
-      <c r="D33" s="87"/>
-      <c r="E33" s="87"/>
+      <c r="D33" s="69"/>
+      <c r="E33" s="69"/>
       <c r="F33" s="40"/>
       <c r="G33" s="40"/>
       <c r="H33" s="40"/>
@@ -7780,7 +7765,7 @@
     </row>
     <row r="34" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A34" s="33">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B34" s="33"/>
       <c r="C34" s="33"/>
@@ -7799,7 +7784,7 @@
     </row>
     <row r="35" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A35" s="33">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B35" s="33"/>
       <c r="C35" s="33"/>
@@ -7818,7 +7803,7 @@
     </row>
     <row r="36" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A36" s="33">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B36" s="33"/>
       <c r="C36" s="33"/>
@@ -7837,7 +7822,7 @@
     </row>
     <row r="37" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A37" s="33">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B37" s="33"/>
       <c r="C37" s="33"/>
@@ -7856,7 +7841,7 @@
     </row>
     <row r="38" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A38" s="33">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B38" s="33"/>
       <c r="C38" s="33"/>
@@ -7875,7 +7860,7 @@
     </row>
     <row r="39" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A39" s="33">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B39" s="33"/>
       <c r="C39" s="33"/>
@@ -7894,7 +7879,7 @@
     </row>
     <row r="40" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A40" s="33">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B40" s="33"/>
       <c r="C40" s="33"/>
@@ -7913,7 +7898,7 @@
     </row>
     <row r="41" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A41" s="33">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B41" s="33"/>
       <c r="C41" s="33"/>
@@ -7932,7 +7917,7 @@
     </row>
     <row r="42" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A42" s="33">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B42" s="33"/>
       <c r="C42" s="33"/>
@@ -7951,7 +7936,7 @@
     </row>
     <row r="43" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A43" s="33">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B43" s="33"/>
       <c r="C43" s="33"/>
@@ -7970,7 +7955,7 @@
     </row>
     <row r="44" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A44" s="33">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B44" s="33"/>
       <c r="C44" s="33"/>
@@ -7989,7 +7974,7 @@
     </row>
     <row r="45" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A45" s="33">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B45" s="33"/>
       <c r="C45" s="33"/>
@@ -8008,7 +7993,7 @@
     </row>
     <row r="46" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A46" s="33">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B46" s="33"/>
       <c r="C46" s="33"/>
@@ -8027,7 +8012,7 @@
     </row>
     <row r="47" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A47" s="33">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B47" s="33"/>
       <c r="C47" s="33"/>
@@ -8046,7 +8031,7 @@
     </row>
     <row r="48" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A48" s="33">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B48" s="33"/>
       <c r="C48" s="33"/>
@@ -8065,7 +8050,7 @@
     </row>
     <row r="49" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A49" s="33">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B49" s="33"/>
       <c r="C49" s="33"/>
@@ -8084,7 +8069,7 @@
     </row>
     <row r="50" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A50" s="33">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B50" s="33"/>
       <c r="C50" s="33"/>
@@ -8103,7 +8088,7 @@
     </row>
     <row r="51" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A51" s="33">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B51" s="33"/>
       <c r="C51" s="33"/>
@@ -8122,13 +8107,13 @@
     </row>
     <row r="52" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A52" s="33">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B52" s="33"/>
       <c r="C52" s="33"/>
-      <c r="D52" s="69"/>
-      <c r="E52" s="69"/>
-      <c r="F52" s="40"/>
+      <c r="D52" s="74"/>
+      <c r="E52" s="74"/>
+      <c r="F52" s="74"/>
       <c r="G52" s="40"/>
       <c r="H52" s="40"/>
       <c r="I52" s="40"/>
@@ -8141,12 +8126,12 @@
     </row>
     <row r="53" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A53" s="33">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B53" s="33"/>
       <c r="C53" s="33"/>
-      <c r="D53" s="69"/>
-      <c r="E53" s="69"/>
+      <c r="D53" s="74"/>
+      <c r="E53" s="74"/>
       <c r="F53" s="40"/>
       <c r="G53" s="40"/>
       <c r="H53" s="40"/>
@@ -8160,13 +8145,13 @@
     </row>
     <row r="54" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A54" s="33">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B54" s="33"/>
       <c r="C54" s="33"/>
-      <c r="D54" s="69"/>
-      <c r="E54" s="69"/>
-      <c r="F54" s="40"/>
+      <c r="D54" s="74"/>
+      <c r="E54" s="74"/>
+      <c r="F54" s="74"/>
       <c r="G54" s="40"/>
       <c r="H54" s="40"/>
       <c r="I54" s="40"/>
@@ -8179,13 +8164,13 @@
     </row>
     <row r="55" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A55" s="33">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B55" s="33"/>
       <c r="C55" s="33"/>
       <c r="D55" s="74"/>
       <c r="E55" s="74"/>
-      <c r="F55" s="74"/>
+      <c r="F55" s="40"/>
       <c r="G55" s="40"/>
       <c r="H55" s="40"/>
       <c r="I55" s="40"/>
@@ -8198,7 +8183,7 @@
     </row>
     <row r="56" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A56" s="33">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B56" s="33"/>
       <c r="C56" s="33"/>
@@ -8217,13 +8202,13 @@
     </row>
     <row r="57" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A57" s="33">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B57" s="33"/>
       <c r="C57" s="33"/>
       <c r="D57" s="74"/>
       <c r="E57" s="74"/>
-      <c r="F57" s="74"/>
+      <c r="F57" s="40"/>
       <c r="G57" s="40"/>
       <c r="H57" s="40"/>
       <c r="I57" s="40"/>
@@ -8236,7 +8221,7 @@
     </row>
     <row r="58" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A58" s="33">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B58" s="33"/>
       <c r="C58" s="33"/>
@@ -8253,63 +8238,6 @@
       <c r="N58" s="61"/>
       <c r="O58" s="32"/>
     </row>
-    <row r="59" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
-      <c r="A59" s="33">
-        <v>48</v>
-      </c>
-      <c r="B59" s="33"/>
-      <c r="C59" s="33"/>
-      <c r="D59" s="74"/>
-      <c r="E59" s="74"/>
-      <c r="F59" s="40"/>
-      <c r="G59" s="40"/>
-      <c r="H59" s="40"/>
-      <c r="I59" s="40"/>
-      <c r="J59" s="61"/>
-      <c r="K59" s="40"/>
-      <c r="L59" s="62"/>
-      <c r="M59" s="61"/>
-      <c r="N59" s="61"/>
-      <c r="O59" s="32"/>
-    </row>
-    <row r="60" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
-      <c r="A60" s="33">
-        <v>49</v>
-      </c>
-      <c r="B60" s="33"/>
-      <c r="C60" s="33"/>
-      <c r="D60" s="74"/>
-      <c r="E60" s="74"/>
-      <c r="F60" s="40"/>
-      <c r="G60" s="40"/>
-      <c r="H60" s="40"/>
-      <c r="I60" s="40"/>
-      <c r="J60" s="61"/>
-      <c r="K60" s="40"/>
-      <c r="L60" s="62"/>
-      <c r="M60" s="61"/>
-      <c r="N60" s="61"/>
-      <c r="O60" s="32"/>
-    </row>
-    <row r="61" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
-      <c r="A61" s="33">
-        <v>50</v>
-      </c>
-      <c r="B61" s="33"/>
-      <c r="C61" s="33"/>
-      <c r="D61" s="74"/>
-      <c r="E61" s="74"/>
-      <c r="F61" s="40"/>
-      <c r="G61" s="40"/>
-      <c r="H61" s="40"/>
-      <c r="I61" s="40"/>
-      <c r="J61" s="61"/>
-      <c r="K61" s="40"/>
-      <c r="L61" s="62"/>
-      <c r="M61" s="61"/>
-      <c r="N61" s="61"/>
-      <c r="O61" s="32"/>
-    </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:D2"/>
@@ -8319,20 +8247,20 @@
     <mergeCell ref="I2:K2"/>
   </mergeCells>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M32:N61 L31:M31">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M29:N58 L28:M28">
       <formula1>"   ,l"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H29:H61 H5:H26">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H26:H58 H5:H23">
       <formula1>"Text, Number, DateTime, Boolean"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="F33:F61 F5"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K5:K61">
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="F30:F58 F5"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G22:G58">
+      <formula1>"Caption,Textbox,DateTimePicker,RichTextbox,Label,ComboBox,CheckBox,RadioButton,Button,DataGrid, Image,Link,Form,Frame,Menu,MenuItem,Other"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K5:K58">
       <formula1>"I,O,I/O"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G25:G61">
-      <formula1>"Caption,Textbox,DateTimePicker,RichTextbox,Label,ComboBox,CheckBox,RadioButton,Button,DataGrid, Image,Link,Form,Frame,Menu,MenuItem,Other"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5:G24">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5:G21">
       <formula1>"Caption,Textbox,DropDownCheckList, DateTimePicker,RichTextbox,Label,ComboBox,CheckBox,RadioButton,Button,DataGrid, Image,Link,Form,Frame,Menu,MenuItem,Other"</formula1>
     </dataValidation>
   </dataValidations>
@@ -8385,7 +8313,7 @@
       </c>
       <c r="E1" s="105" t="str">
         <f>'Update History'!F1</f>
-        <v>CRMFXXX1</v>
+        <v>CRMF3010</v>
       </c>
       <c r="F1" s="30" t="s">
         <v>5</v>
@@ -9310,8 +9238,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R56"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6:G6"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1"/>
@@ -9351,7 +9279,7 @@
       </c>
       <c r="F1" s="102" t="str">
         <f>'Update History'!F1</f>
-        <v>CRMFXXX1</v>
+        <v>CRMF3010</v>
       </c>
       <c r="G1" s="103" t="s">
         <v>5</v>
@@ -9424,7 +9352,7 @@
       <c r="I4" s="163"/>
       <c r="J4" s="163"/>
     </row>
-    <row r="5" spans="1:12" s="34" customFormat="1" ht="11.25">
+    <row r="5" spans="1:12" s="34" customFormat="1" ht="27" customHeight="1">
       <c r="A5" s="33">
         <v>1</v>
       </c>
@@ -9433,15 +9361,15 @@
       </c>
       <c r="C5" s="33"/>
       <c r="D5" s="131" t="s">
-        <v>134</v>
+        <v>233</v>
       </c>
       <c r="E5" s="32"/>
       <c r="F5" s="190" t="s">
-        <v>184</v>
+        <v>238</v>
       </c>
       <c r="G5" s="191"/>
       <c r="H5" s="194" t="s">
-        <v>185</v>
+        <v>234</v>
       </c>
       <c r="I5" s="195"/>
       <c r="J5" s="196"/>
@@ -9459,11 +9387,11 @@
       </c>
       <c r="E6" s="32"/>
       <c r="F6" s="190" t="s">
-        <v>206</v>
+        <v>227</v>
       </c>
       <c r="G6" s="191"/>
       <c r="H6" s="194" t="s">
-        <v>205</v>
+        <v>183</v>
       </c>
       <c r="I6" s="195"/>
       <c r="J6" s="196"/>
@@ -10468,10 +10396,1118 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J87"/>
+  <sheetViews>
+    <sheetView view="pageBreakPreview" topLeftCell="A7" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" style="22" customWidth="1"/>
+    <col min="2" max="2" width="3.85546875" style="22" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" style="22" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" style="22" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" style="22" customWidth="1"/>
+    <col min="6" max="6" width="31.7109375" style="22" customWidth="1"/>
+    <col min="7" max="10" width="12.7109375" style="22" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="22"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="12" customHeight="1">
+      <c r="A1" s="163" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="163"/>
+      <c r="C1" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="36" t="str">
+        <f>'Update History'!D1</f>
+        <v>ASOFT - ERP.NET</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="36" t="str">
+        <f>'Update History'!F1</f>
+        <v>CRMF3010</v>
+      </c>
+      <c r="G1" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="37" t="str">
+        <f>'Update History'!H1</f>
+        <v>Thị Phượng</v>
+      </c>
+      <c r="I1" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="67" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="12" customHeight="1">
+      <c r="A2" s="163"/>
+      <c r="B2" s="163"/>
+      <c r="C2" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="36" t="str">
+        <f>'Update History'!D2</f>
+        <v>ASOFT - CRM</v>
+      </c>
+      <c r="E2" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="36" t="str">
+        <f>'Update History'!F2</f>
+        <v>Báo cáo Khách hàng mới theo nhân viên</v>
+      </c>
+      <c r="G2" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="38">
+        <f>'Update History'!H2</f>
+        <v>42396</v>
+      </c>
+      <c r="I2" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="67">
+        <v>42396</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="12" customHeight="1">
+      <c r="A4" s="54"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="56"/>
+    </row>
+    <row r="5" spans="1:10" ht="12" customHeight="1">
+      <c r="A5" s="73" t="s">
+        <v>112</v>
+      </c>
+      <c r="B5" s="43"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="46"/>
+    </row>
+    <row r="6" spans="1:10" ht="12" customHeight="1">
+      <c r="A6" s="42"/>
+      <c r="B6" s="43"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="46"/>
+    </row>
+    <row r="7" spans="1:10" ht="12" customHeight="1">
+      <c r="A7" s="42"/>
+      <c r="B7" s="43"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="43"/>
+      <c r="J7" s="46"/>
+    </row>
+    <row r="8" spans="1:10" ht="12" customHeight="1">
+      <c r="A8" s="73" t="s">
+        <v>115</v>
+      </c>
+      <c r="B8" s="43"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="46"/>
+    </row>
+    <row r="9" spans="1:10" ht="12" customHeight="1">
+      <c r="A9" s="80"/>
+      <c r="B9" s="80" t="s">
+        <v>156</v>
+      </c>
+      <c r="C9" s="43"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="43"/>
+      <c r="J9" s="46"/>
+    </row>
+    <row r="10" spans="1:10" ht="12" customHeight="1">
+      <c r="A10" s="80"/>
+      <c r="B10" s="43"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="46"/>
+    </row>
+    <row r="11" spans="1:10" ht="12" customHeight="1">
+      <c r="A11" s="80"/>
+      <c r="B11" s="80" t="s">
+        <v>116</v>
+      </c>
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="46"/>
+    </row>
+    <row r="12" spans="1:10" ht="12" customHeight="1">
+      <c r="A12" s="80"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="46"/>
+    </row>
+    <row r="13" spans="1:10" ht="12" customHeight="1">
+      <c r="A13" s="80"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="46"/>
+    </row>
+    <row r="14" spans="1:10" ht="12" customHeight="1">
+      <c r="B14" s="80" t="s">
+        <v>117</v>
+      </c>
+      <c r="C14" s="43"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="43"/>
+      <c r="J14" s="46"/>
+    </row>
+    <row r="16" spans="1:10" ht="12" customHeight="1">
+      <c r="B16" s="80" t="s">
+        <v>118</v>
+      </c>
+      <c r="C16" s="43"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="43"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="43"/>
+      <c r="H16" s="43"/>
+      <c r="I16" s="43"/>
+      <c r="J16" s="46"/>
+    </row>
+    <row r="17" spans="1:10" ht="12" customHeight="1">
+      <c r="B17" s="43"/>
+      <c r="C17" s="43" t="s">
+        <v>208</v>
+      </c>
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="43"/>
+      <c r="I17" s="43"/>
+      <c r="J17" s="46"/>
+    </row>
+    <row r="18" spans="1:10" ht="12" customHeight="1">
+      <c r="B18" s="43"/>
+      <c r="C18" s="43"/>
+      <c r="D18" s="43"/>
+      <c r="E18" s="43"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="43"/>
+      <c r="H18" s="43"/>
+      <c r="I18" s="43"/>
+      <c r="J18" s="46"/>
+    </row>
+    <row r="19" spans="1:10" ht="12" customHeight="1">
+      <c r="B19" s="80" t="s">
+        <v>119</v>
+      </c>
+      <c r="C19" s="43"/>
+      <c r="D19" s="43"/>
+      <c r="E19" s="43"/>
+      <c r="F19" s="43"/>
+      <c r="G19" s="43"/>
+      <c r="H19" s="43"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="46"/>
+    </row>
+    <row r="20" spans="1:10" ht="12" customHeight="1">
+      <c r="B20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="43"/>
+      <c r="J20" s="46"/>
+    </row>
+    <row r="21" spans="1:10" ht="12" customHeight="1">
+      <c r="B21" s="43"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="43"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="43"/>
+      <c r="I21" s="43"/>
+      <c r="J21" s="46"/>
+    </row>
+    <row r="22" spans="1:10" ht="12" customHeight="1">
+      <c r="B22" s="80" t="s">
+        <v>120</v>
+      </c>
+      <c r="C22" s="43"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="43"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="43"/>
+      <c r="H22" s="43"/>
+      <c r="I22" s="43"/>
+      <c r="J22" s="46"/>
+    </row>
+    <row r="23" spans="1:10" ht="12" customHeight="1">
+      <c r="B23" s="80"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="43"/>
+      <c r="G23" s="43"/>
+      <c r="H23" s="43"/>
+      <c r="I23" s="43"/>
+      <c r="J23" s="46"/>
+    </row>
+    <row r="24" spans="1:10" ht="12" customHeight="1">
+      <c r="A24" s="42"/>
+      <c r="B24" s="43"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="43"/>
+      <c r="G24" s="43"/>
+      <c r="H24" s="43"/>
+      <c r="I24" s="43"/>
+      <c r="J24" s="46"/>
+    </row>
+    <row r="25" spans="1:10" ht="12" customHeight="1">
+      <c r="A25" s="73" t="s">
+        <v>114</v>
+      </c>
+      <c r="B25" s="43"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="43"/>
+      <c r="E25" s="43"/>
+      <c r="F25" s="43"/>
+      <c r="G25" s="43"/>
+      <c r="H25" s="43"/>
+      <c r="I25" s="43"/>
+      <c r="J25" s="46"/>
+    </row>
+    <row r="26" spans="1:10" ht="12" customHeight="1">
+      <c r="A26" s="73"/>
+      <c r="B26" s="43" t="s">
+        <v>236</v>
+      </c>
+      <c r="C26" s="43"/>
+      <c r="D26" s="43"/>
+      <c r="E26" s="43"/>
+      <c r="F26" s="43"/>
+      <c r="G26" s="43"/>
+      <c r="H26" s="43"/>
+      <c r="I26" s="43"/>
+      <c r="J26" s="46"/>
+    </row>
+    <row r="27" spans="1:10" ht="12" customHeight="1">
+      <c r="A27" s="42"/>
+      <c r="B27" s="86"/>
+      <c r="C27" s="86"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="43"/>
+      <c r="F27" s="43"/>
+      <c r="G27" s="43"/>
+      <c r="H27" s="43"/>
+      <c r="I27" s="43"/>
+      <c r="J27" s="46"/>
+    </row>
+    <row r="28" spans="1:10" ht="12" customHeight="1">
+      <c r="A28" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="B28" s="43"/>
+      <c r="C28" s="86"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="46"/>
+    </row>
+    <row r="29" spans="1:10" ht="12" customHeight="1">
+      <c r="B29" s="80" t="s">
+        <v>121</v>
+      </c>
+      <c r="C29" s="86"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="43"/>
+      <c r="G29" s="43"/>
+      <c r="H29" s="43"/>
+      <c r="I29" s="43"/>
+      <c r="J29" s="46"/>
+    </row>
+    <row r="30" spans="1:10" ht="12" customHeight="1">
+      <c r="B30" s="43"/>
+      <c r="C30" s="86"/>
+      <c r="D30" s="43"/>
+      <c r="E30" s="43"/>
+      <c r="F30" s="43"/>
+      <c r="G30" s="43"/>
+      <c r="H30" s="43"/>
+      <c r="I30" s="43"/>
+      <c r="J30" s="46"/>
+    </row>
+    <row r="31" spans="1:10" ht="12" customHeight="1">
+      <c r="B31" s="43"/>
+      <c r="C31" s="86"/>
+      <c r="D31" s="43"/>
+      <c r="E31" s="43"/>
+      <c r="F31" s="43"/>
+      <c r="G31" s="43"/>
+      <c r="H31" s="43"/>
+      <c r="I31" s="43"/>
+      <c r="J31" s="46"/>
+    </row>
+    <row r="32" spans="1:10" ht="12" customHeight="1">
+      <c r="B32" s="80" t="s">
+        <v>122</v>
+      </c>
+      <c r="C32" s="43"/>
+      <c r="D32" s="43"/>
+      <c r="E32" s="43"/>
+      <c r="F32" s="43"/>
+      <c r="G32" s="43"/>
+      <c r="H32" s="43"/>
+      <c r="I32" s="43"/>
+      <c r="J32" s="46"/>
+    </row>
+    <row r="33" spans="1:10" ht="12" customHeight="1">
+      <c r="B33" s="80"/>
+      <c r="C33" s="86"/>
+      <c r="D33" s="43"/>
+      <c r="E33" s="43"/>
+      <c r="F33" s="43"/>
+      <c r="G33" s="43"/>
+      <c r="H33" s="43"/>
+      <c r="I33" s="43"/>
+      <c r="J33" s="46"/>
+    </row>
+    <row r="34" spans="1:10" ht="12" customHeight="1">
+      <c r="A34" s="42"/>
+      <c r="B34" s="43"/>
+      <c r="C34" s="43"/>
+      <c r="D34" s="43"/>
+      <c r="E34" s="43"/>
+      <c r="F34" s="43"/>
+      <c r="G34" s="43"/>
+      <c r="H34" s="43"/>
+      <c r="I34" s="43"/>
+      <c r="J34" s="46"/>
+    </row>
+    <row r="35" spans="1:10" ht="12" customHeight="1">
+      <c r="A35" s="73" t="s">
+        <v>124</v>
+      </c>
+      <c r="B35" s="43"/>
+      <c r="C35" s="86"/>
+      <c r="D35" s="43"/>
+      <c r="E35" s="43"/>
+      <c r="F35" s="43"/>
+      <c r="G35" s="43"/>
+      <c r="H35" s="43"/>
+      <c r="I35" s="43"/>
+      <c r="J35" s="46"/>
+    </row>
+    <row r="36" spans="1:10" ht="12" customHeight="1">
+      <c r="B36" s="80" t="s">
+        <v>121</v>
+      </c>
+      <c r="C36" s="86"/>
+      <c r="D36" s="43"/>
+      <c r="E36" s="43"/>
+      <c r="F36" s="43"/>
+      <c r="G36" s="43"/>
+      <c r="H36" s="43"/>
+      <c r="I36" s="43"/>
+      <c r="J36" s="46"/>
+    </row>
+    <row r="37" spans="1:10" ht="12" customHeight="1">
+      <c r="B37" s="43"/>
+      <c r="C37" s="86"/>
+      <c r="D37" s="43"/>
+      <c r="E37" s="43"/>
+      <c r="F37" s="43"/>
+      <c r="G37" s="43"/>
+      <c r="H37" s="43"/>
+      <c r="I37" s="43"/>
+      <c r="J37" s="46"/>
+    </row>
+    <row r="38" spans="1:10" ht="12" customHeight="1">
+      <c r="B38" s="43"/>
+      <c r="C38" s="86"/>
+      <c r="D38" s="43"/>
+      <c r="E38" s="43"/>
+      <c r="F38" s="43"/>
+      <c r="G38" s="43"/>
+      <c r="H38" s="43"/>
+      <c r="I38" s="43"/>
+      <c r="J38" s="46"/>
+    </row>
+    <row r="39" spans="1:10" ht="12" customHeight="1">
+      <c r="B39" s="80" t="s">
+        <v>122</v>
+      </c>
+      <c r="C39" s="43"/>
+      <c r="D39" s="43"/>
+      <c r="E39" s="43"/>
+      <c r="F39" s="43"/>
+      <c r="G39" s="43"/>
+      <c r="H39" s="43"/>
+      <c r="I39" s="43"/>
+      <c r="J39" s="46"/>
+    </row>
+    <row r="40" spans="1:10" ht="12" customHeight="1">
+      <c r="B40" s="80"/>
+      <c r="C40" s="86"/>
+      <c r="D40" s="43"/>
+      <c r="E40" s="43"/>
+      <c r="F40" s="43"/>
+      <c r="G40" s="43"/>
+      <c r="H40" s="43"/>
+      <c r="I40" s="43"/>
+      <c r="J40" s="46"/>
+    </row>
+    <row r="41" spans="1:10" ht="12" customHeight="1">
+      <c r="A41" s="42"/>
+      <c r="B41" s="86"/>
+      <c r="C41" s="43"/>
+      <c r="D41" s="43"/>
+      <c r="E41" s="43"/>
+      <c r="F41" s="43"/>
+      <c r="G41" s="43"/>
+      <c r="H41" s="43"/>
+      <c r="I41" s="43"/>
+      <c r="J41" s="46"/>
+    </row>
+    <row r="42" spans="1:10" ht="12" customHeight="1">
+      <c r="A42" s="73" t="s">
+        <v>125</v>
+      </c>
+      <c r="B42" s="43"/>
+      <c r="C42" s="86"/>
+      <c r="D42" s="43"/>
+      <c r="E42" s="43"/>
+      <c r="F42" s="43"/>
+      <c r="G42" s="43"/>
+      <c r="H42" s="43"/>
+      <c r="I42" s="43"/>
+      <c r="J42" s="46"/>
+    </row>
+    <row r="43" spans="1:10" ht="12" customHeight="1">
+      <c r="B43" s="80" t="s">
+        <v>126</v>
+      </c>
+      <c r="C43" s="86"/>
+      <c r="D43" s="43"/>
+      <c r="E43" s="43"/>
+      <c r="F43" s="43"/>
+      <c r="G43" s="43"/>
+      <c r="H43" s="43"/>
+      <c r="I43" s="43"/>
+      <c r="J43" s="46"/>
+    </row>
+    <row r="44" spans="1:10" ht="12" customHeight="1">
+      <c r="B44" s="80"/>
+      <c r="C44" s="86"/>
+      <c r="D44" s="43"/>
+      <c r="E44" s="43"/>
+      <c r="F44" s="43"/>
+      <c r="G44" s="43"/>
+      <c r="H44" s="43"/>
+      <c r="I44" s="43"/>
+      <c r="J44" s="46"/>
+    </row>
+    <row r="45" spans="1:10" ht="12" customHeight="1">
+      <c r="B45" s="43"/>
+      <c r="C45" s="86"/>
+      <c r="D45" s="43"/>
+      <c r="E45" s="43"/>
+      <c r="F45" s="43"/>
+      <c r="G45" s="43"/>
+      <c r="H45" s="43"/>
+      <c r="I45" s="43"/>
+      <c r="J45" s="46"/>
+    </row>
+    <row r="46" spans="1:10" ht="12" customHeight="1">
+      <c r="B46" s="80" t="s">
+        <v>127</v>
+      </c>
+      <c r="C46" s="43"/>
+      <c r="D46" s="43"/>
+      <c r="E46" s="43"/>
+      <c r="F46" s="43"/>
+      <c r="G46" s="43"/>
+      <c r="H46" s="43"/>
+      <c r="I46" s="43"/>
+      <c r="J46" s="46"/>
+    </row>
+    <row r="47" spans="1:10" ht="12" customHeight="1">
+      <c r="B47" s="80"/>
+      <c r="C47" s="43"/>
+      <c r="D47" s="43"/>
+      <c r="E47" s="43"/>
+      <c r="F47" s="43"/>
+      <c r="G47" s="43"/>
+      <c r="H47" s="43"/>
+      <c r="I47" s="43"/>
+      <c r="J47" s="46"/>
+    </row>
+    <row r="48" spans="1:10" ht="12" customHeight="1">
+      <c r="A48" s="73" t="s">
+        <v>128</v>
+      </c>
+      <c r="B48" s="43"/>
+      <c r="C48" s="86"/>
+      <c r="D48" s="43"/>
+      <c r="E48" s="43"/>
+      <c r="F48" s="43"/>
+      <c r="G48" s="43"/>
+      <c r="H48" s="43"/>
+      <c r="I48" s="43"/>
+      <c r="J48" s="46"/>
+    </row>
+    <row r="49" spans="1:10" ht="12" customHeight="1">
+      <c r="B49" s="80" t="s">
+        <v>197</v>
+      </c>
+      <c r="C49" s="86"/>
+      <c r="D49" s="43"/>
+      <c r="E49" s="43"/>
+      <c r="F49" s="43"/>
+      <c r="G49" s="43"/>
+      <c r="H49" s="43"/>
+      <c r="I49" s="43"/>
+      <c r="J49" s="46"/>
+    </row>
+    <row r="50" spans="1:10" ht="12" customHeight="1">
+      <c r="B50" s="43"/>
+      <c r="C50" s="86"/>
+      <c r="D50" s="43"/>
+      <c r="E50" s="43"/>
+      <c r="F50" s="43"/>
+      <c r="G50" s="43"/>
+      <c r="H50" s="43"/>
+      <c r="I50" s="43"/>
+      <c r="J50" s="46"/>
+    </row>
+    <row r="51" spans="1:10" ht="12" customHeight="1">
+      <c r="B51" s="80"/>
+      <c r="C51" s="43"/>
+      <c r="D51" s="43"/>
+      <c r="E51" s="43"/>
+      <c r="F51" s="43"/>
+      <c r="G51" s="43"/>
+      <c r="H51" s="43"/>
+      <c r="I51" s="43"/>
+      <c r="J51" s="46"/>
+    </row>
+    <row r="52" spans="1:10" ht="12" customHeight="1">
+      <c r="B52" s="80"/>
+      <c r="C52" s="43"/>
+      <c r="D52" s="43"/>
+      <c r="E52" s="43"/>
+      <c r="F52" s="43"/>
+      <c r="G52" s="43"/>
+      <c r="H52" s="43"/>
+      <c r="I52" s="43"/>
+      <c r="J52" s="46"/>
+    </row>
+    <row r="53" spans="1:10" ht="12" customHeight="1">
+      <c r="B53" s="43"/>
+      <c r="C53" s="43"/>
+      <c r="D53" s="43"/>
+      <c r="E53" s="43"/>
+      <c r="F53" s="43"/>
+      <c r="G53" s="43"/>
+      <c r="H53" s="43"/>
+      <c r="I53" s="43"/>
+      <c r="J53" s="46"/>
+    </row>
+    <row r="54" spans="1:10" ht="12" customHeight="1">
+      <c r="B54" s="43"/>
+      <c r="C54" s="43"/>
+      <c r="D54" s="43"/>
+      <c r="E54" s="43"/>
+      <c r="F54" s="43"/>
+      <c r="G54" s="43"/>
+      <c r="H54" s="43"/>
+      <c r="I54" s="43"/>
+      <c r="J54" s="46"/>
+    </row>
+    <row r="55" spans="1:10" ht="12" customHeight="1">
+      <c r="B55" s="80"/>
+      <c r="C55" s="43"/>
+      <c r="D55" s="43"/>
+      <c r="E55" s="43"/>
+      <c r="F55" s="43"/>
+      <c r="G55" s="43"/>
+      <c r="H55" s="43"/>
+      <c r="I55" s="43"/>
+      <c r="J55" s="46"/>
+    </row>
+    <row r="56" spans="1:10" ht="12" customHeight="1">
+      <c r="A56" s="42"/>
+      <c r="B56" s="43"/>
+      <c r="C56" s="86"/>
+      <c r="D56" s="43"/>
+      <c r="E56" s="43"/>
+      <c r="F56" s="43"/>
+      <c r="G56" s="43"/>
+      <c r="H56" s="43"/>
+      <c r="I56" s="43"/>
+      <c r="J56" s="46"/>
+    </row>
+    <row r="57" spans="1:10" ht="12" customHeight="1">
+      <c r="A57" s="42"/>
+      <c r="B57" s="43"/>
+      <c r="C57" s="86"/>
+      <c r="D57" s="43"/>
+      <c r="E57" s="43"/>
+      <c r="F57" s="43"/>
+      <c r="G57" s="43"/>
+      <c r="H57" s="43"/>
+      <c r="I57" s="43"/>
+      <c r="J57" s="46"/>
+    </row>
+    <row r="58" spans="1:10" ht="12" customHeight="1">
+      <c r="A58" s="42"/>
+      <c r="B58" s="43"/>
+      <c r="C58" s="86"/>
+      <c r="D58" s="43"/>
+      <c r="E58" s="43"/>
+      <c r="F58" s="43"/>
+      <c r="G58" s="43"/>
+      <c r="H58" s="43"/>
+      <c r="I58" s="43"/>
+      <c r="J58" s="46"/>
+    </row>
+    <row r="59" spans="1:10" ht="12" customHeight="1">
+      <c r="A59" s="73"/>
+      <c r="B59" s="43"/>
+      <c r="C59" s="43"/>
+      <c r="D59" s="43"/>
+      <c r="E59" s="43"/>
+      <c r="F59" s="43"/>
+      <c r="G59" s="43"/>
+      <c r="H59" s="43"/>
+      <c r="I59" s="43"/>
+      <c r="J59" s="46"/>
+    </row>
+    <row r="60" spans="1:10" ht="12" customHeight="1">
+      <c r="B60" s="80"/>
+      <c r="C60" s="43"/>
+      <c r="D60" s="43"/>
+      <c r="E60" s="43"/>
+      <c r="F60" s="43"/>
+      <c r="G60" s="43"/>
+      <c r="H60" s="43"/>
+      <c r="I60" s="43"/>
+      <c r="J60" s="46"/>
+    </row>
+    <row r="61" spans="1:10" ht="12" customHeight="1">
+      <c r="B61" s="43"/>
+      <c r="C61" s="43"/>
+      <c r="D61" s="43"/>
+      <c r="E61" s="43"/>
+      <c r="F61" s="43"/>
+      <c r="G61" s="43"/>
+      <c r="H61" s="43"/>
+      <c r="I61" s="43"/>
+      <c r="J61" s="46"/>
+    </row>
+    <row r="62" spans="1:10" ht="12" customHeight="1">
+      <c r="B62" s="80"/>
+      <c r="C62" s="43"/>
+      <c r="D62" s="43"/>
+      <c r="E62" s="43"/>
+      <c r="F62" s="43"/>
+      <c r="G62" s="43"/>
+      <c r="H62" s="43"/>
+      <c r="I62" s="43"/>
+      <c r="J62" s="46"/>
+    </row>
+    <row r="63" spans="1:10" ht="12" customHeight="1">
+      <c r="A63" s="42"/>
+      <c r="B63" s="43"/>
+      <c r="C63" s="43"/>
+      <c r="D63" s="43"/>
+      <c r="E63" s="43"/>
+      <c r="F63" s="43"/>
+      <c r="G63" s="43"/>
+      <c r="H63" s="43"/>
+      <c r="I63" s="43"/>
+      <c r="J63" s="46"/>
+    </row>
+    <row r="64" spans="1:10" ht="12" customHeight="1">
+      <c r="A64" s="73"/>
+      <c r="B64" s="43"/>
+      <c r="C64" s="43"/>
+      <c r="D64" s="43"/>
+      <c r="E64" s="43"/>
+      <c r="F64" s="43"/>
+      <c r="G64" s="43"/>
+      <c r="H64" s="43"/>
+      <c r="I64" s="43"/>
+      <c r="J64" s="46"/>
+    </row>
+    <row r="65" spans="1:10" ht="12" customHeight="1">
+      <c r="A65" s="42"/>
+      <c r="B65" s="43"/>
+      <c r="C65" s="43"/>
+      <c r="D65" s="43"/>
+      <c r="E65" s="43"/>
+      <c r="F65" s="43"/>
+      <c r="G65" s="43"/>
+      <c r="H65" s="43"/>
+      <c r="I65" s="43"/>
+      <c r="J65" s="46"/>
+    </row>
+    <row r="66" spans="1:10" ht="12" customHeight="1">
+      <c r="A66" s="42"/>
+      <c r="B66" s="43"/>
+      <c r="C66" s="43"/>
+      <c r="D66" s="43"/>
+      <c r="E66" s="43"/>
+      <c r="F66" s="43"/>
+      <c r="G66" s="43"/>
+      <c r="H66" s="43"/>
+      <c r="I66" s="43"/>
+      <c r="J66" s="46"/>
+    </row>
+    <row r="67" spans="1:10" ht="12" customHeight="1">
+      <c r="A67" s="42"/>
+      <c r="B67" s="43"/>
+      <c r="C67" s="43"/>
+      <c r="D67" s="43"/>
+      <c r="E67" s="43"/>
+      <c r="F67" s="43"/>
+      <c r="G67" s="43"/>
+      <c r="H67" s="43"/>
+      <c r="I67" s="43"/>
+      <c r="J67" s="46"/>
+    </row>
+    <row r="68" spans="1:10" ht="12" customHeight="1">
+      <c r="A68" s="42"/>
+      <c r="B68" s="43"/>
+      <c r="C68" s="43"/>
+      <c r="D68" s="43"/>
+      <c r="E68" s="43"/>
+      <c r="F68" s="43"/>
+      <c r="G68" s="43"/>
+      <c r="H68" s="43"/>
+      <c r="I68" s="43"/>
+      <c r="J68" s="46"/>
+    </row>
+    <row r="69" spans="1:10" ht="12" customHeight="1">
+      <c r="A69" s="42"/>
+      <c r="B69" s="43"/>
+      <c r="C69" s="43"/>
+      <c r="D69" s="43"/>
+      <c r="E69" s="43"/>
+      <c r="F69" s="43"/>
+      <c r="G69" s="43"/>
+      <c r="H69" s="43"/>
+      <c r="I69" s="43"/>
+      <c r="J69" s="46"/>
+    </row>
+    <row r="70" spans="1:10" ht="12" customHeight="1">
+      <c r="A70" s="42"/>
+      <c r="B70" s="43"/>
+      <c r="C70" s="43"/>
+      <c r="D70" s="43"/>
+      <c r="E70" s="43"/>
+      <c r="F70" s="43"/>
+      <c r="G70" s="43"/>
+      <c r="H70" s="43"/>
+      <c r="I70" s="43"/>
+      <c r="J70" s="46"/>
+    </row>
+    <row r="71" spans="1:10" ht="12" customHeight="1">
+      <c r="A71" s="42"/>
+      <c r="B71" s="43"/>
+      <c r="C71" s="43"/>
+      <c r="D71" s="43"/>
+      <c r="E71" s="43"/>
+      <c r="F71" s="43"/>
+      <c r="G71" s="43"/>
+      <c r="H71" s="43"/>
+      <c r="I71" s="43"/>
+      <c r="J71" s="46"/>
+    </row>
+    <row r="72" spans="1:10" ht="12" customHeight="1">
+      <c r="A72" s="42"/>
+      <c r="B72" s="43"/>
+      <c r="C72" s="43"/>
+      <c r="D72" s="43"/>
+      <c r="E72" s="43"/>
+      <c r="F72" s="43"/>
+      <c r="G72" s="43"/>
+      <c r="H72" s="43"/>
+      <c r="I72" s="43"/>
+      <c r="J72" s="46"/>
+    </row>
+    <row r="73" spans="1:10" ht="12" customHeight="1">
+      <c r="A73" s="42"/>
+      <c r="B73" s="43"/>
+      <c r="C73" s="43"/>
+      <c r="D73" s="43"/>
+      <c r="E73" s="43"/>
+      <c r="F73" s="43"/>
+      <c r="G73" s="43"/>
+      <c r="H73" s="43"/>
+      <c r="I73" s="43"/>
+      <c r="J73" s="46"/>
+    </row>
+    <row r="74" spans="1:10" ht="12" customHeight="1">
+      <c r="A74" s="42"/>
+      <c r="B74" s="43"/>
+      <c r="C74" s="43"/>
+      <c r="D74" s="43"/>
+      <c r="E74" s="43"/>
+      <c r="F74" s="43"/>
+      <c r="G74" s="43"/>
+      <c r="H74" s="43"/>
+      <c r="I74" s="43"/>
+      <c r="J74" s="46"/>
+    </row>
+    <row r="75" spans="1:10" ht="12" customHeight="1">
+      <c r="A75" s="42"/>
+      <c r="B75" s="43"/>
+      <c r="C75" s="43"/>
+      <c r="D75" s="43"/>
+      <c r="E75" s="43"/>
+      <c r="F75" s="43"/>
+      <c r="G75" s="43"/>
+      <c r="H75" s="43"/>
+      <c r="I75" s="43"/>
+      <c r="J75" s="46"/>
+    </row>
+    <row r="76" spans="1:10" ht="12" customHeight="1">
+      <c r="A76" s="42"/>
+      <c r="B76" s="43"/>
+      <c r="C76" s="43"/>
+      <c r="D76" s="43"/>
+      <c r="E76" s="43"/>
+      <c r="F76" s="43"/>
+      <c r="G76" s="43"/>
+      <c r="H76" s="43"/>
+      <c r="I76" s="43"/>
+      <c r="J76" s="46"/>
+    </row>
+    <row r="77" spans="1:10" ht="12" customHeight="1">
+      <c r="A77" s="42"/>
+      <c r="B77" s="43"/>
+      <c r="C77" s="43"/>
+      <c r="D77" s="43"/>
+      <c r="E77" s="43"/>
+      <c r="F77" s="43"/>
+      <c r="G77" s="43"/>
+      <c r="H77" s="43"/>
+      <c r="I77" s="43"/>
+      <c r="J77" s="46"/>
+    </row>
+    <row r="78" spans="1:10" ht="12" customHeight="1">
+      <c r="A78" s="42"/>
+      <c r="B78" s="43"/>
+      <c r="C78" s="43"/>
+      <c r="D78" s="43"/>
+      <c r="E78" s="43"/>
+      <c r="F78" s="43"/>
+      <c r="G78" s="43"/>
+      <c r="H78" s="43"/>
+      <c r="I78" s="43"/>
+      <c r="J78" s="46"/>
+    </row>
+    <row r="79" spans="1:10" ht="12" customHeight="1">
+      <c r="A79" s="42"/>
+      <c r="B79" s="43"/>
+      <c r="C79" s="43"/>
+      <c r="D79" s="43"/>
+      <c r="E79" s="43"/>
+      <c r="F79" s="43"/>
+      <c r="G79" s="43"/>
+      <c r="H79" s="43"/>
+      <c r="I79" s="43"/>
+      <c r="J79" s="46"/>
+    </row>
+    <row r="80" spans="1:10" ht="12" customHeight="1">
+      <c r="A80" s="42"/>
+      <c r="B80" s="43"/>
+      <c r="C80" s="43"/>
+      <c r="D80" s="43"/>
+      <c r="E80" s="43"/>
+      <c r="F80" s="43"/>
+      <c r="G80" s="43"/>
+      <c r="H80" s="43"/>
+      <c r="I80" s="43"/>
+      <c r="J80" s="46"/>
+    </row>
+    <row r="81" spans="1:10" ht="12" customHeight="1">
+      <c r="A81" s="42"/>
+      <c r="B81" s="43"/>
+      <c r="C81" s="43"/>
+      <c r="D81" s="43"/>
+      <c r="E81" s="43"/>
+      <c r="F81" s="43"/>
+      <c r="G81" s="43"/>
+      <c r="H81" s="43"/>
+      <c r="I81" s="43"/>
+      <c r="J81" s="46"/>
+    </row>
+    <row r="82" spans="1:10" ht="12" customHeight="1">
+      <c r="A82" s="42"/>
+      <c r="B82" s="43"/>
+      <c r="C82" s="43"/>
+      <c r="D82" s="43"/>
+      <c r="E82" s="43"/>
+      <c r="F82" s="43"/>
+      <c r="G82" s="43"/>
+      <c r="H82" s="43"/>
+      <c r="I82" s="43"/>
+      <c r="J82" s="46"/>
+    </row>
+    <row r="83" spans="1:10" ht="12" customHeight="1">
+      <c r="A83" s="42"/>
+      <c r="B83" s="43"/>
+      <c r="C83" s="43"/>
+      <c r="D83" s="43"/>
+      <c r="E83" s="43"/>
+      <c r="F83" s="43"/>
+      <c r="G83" s="43"/>
+      <c r="H83" s="43"/>
+      <c r="I83" s="43"/>
+      <c r="J83" s="46"/>
+    </row>
+    <row r="84" spans="1:10" ht="12" customHeight="1">
+      <c r="A84" s="42"/>
+      <c r="B84" s="43"/>
+      <c r="C84" s="43"/>
+      <c r="D84" s="43"/>
+      <c r="E84" s="43"/>
+      <c r="F84" s="43"/>
+      <c r="G84" s="43"/>
+      <c r="H84" s="43"/>
+      <c r="I84" s="43"/>
+      <c r="J84" s="46"/>
+    </row>
+    <row r="85" spans="1:10" ht="12" customHeight="1">
+      <c r="A85" s="42"/>
+      <c r="B85" s="43"/>
+      <c r="C85" s="43"/>
+      <c r="D85" s="43"/>
+      <c r="E85" s="43"/>
+      <c r="F85" s="43"/>
+      <c r="G85" s="43"/>
+      <c r="H85" s="43"/>
+      <c r="I85" s="43"/>
+      <c r="J85" s="46"/>
+    </row>
+    <row r="86" spans="1:10" ht="12" customHeight="1">
+      <c r="A86" s="42"/>
+      <c r="B86" s="43"/>
+      <c r="C86" s="43"/>
+      <c r="D86" s="43"/>
+      <c r="E86" s="43"/>
+      <c r="F86" s="43"/>
+      <c r="G86" s="43"/>
+      <c r="H86" s="43"/>
+      <c r="I86" s="43"/>
+      <c r="J86" s="46"/>
+    </row>
+    <row r="87" spans="1:10" ht="12" customHeight="1">
+      <c r="A87" s="47"/>
+      <c r="B87" s="48"/>
+      <c r="C87" s="48"/>
+      <c r="D87" s="48"/>
+      <c r="E87" s="48"/>
+      <c r="F87" s="48"/>
+      <c r="G87" s="48"/>
+      <c r="H87" s="48"/>
+      <c r="I87" s="48"/>
+      <c r="J87" s="57"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B2"/>
+  </mergeCells>
+  <pageMargins left="0.3" right="0.3" top="0.6" bottom="0.3" header="0.1" footer="0.1"/>
+  <pageSetup paperSize="9" scale="81" orientation="landscape" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;R&amp;G</oddHeader>
+    <oddFooter>&amp;L&amp;"Ta,Regular"&amp;10CONFIDENTIAL&amp;C&amp;"Tahoma,Regular"&amp;10&amp;P&amp;R&amp;"Tahoma,Regular"&amp;10© 2010 ASOFT JSC. All rights reserved.</oddFooter>
+  </headerFooter>
+  <rowBreaks count="2" manualBreakCount="2">
+    <brk id="52" max="9" man="1"/>
+    <brk id="65" max="9" man="1"/>
+  </rowBreaks>
+  <legacyDrawing r:id="rId2"/>
+  <legacyDrawingHF r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T1048467"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1"/>
@@ -10521,7 +11557,7 @@
       </c>
       <c r="L1" s="53" t="str">
         <f>'Update History'!F1</f>
-        <v>CRMFXXX1</v>
+        <v>CRMF3010</v>
       </c>
       <c r="M1" s="26" t="s">
         <v>5</v>
@@ -10640,42 +11676,42 @@
         <v>164</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D5" s="33"/>
       <c r="E5" s="32"/>
       <c r="F5" s="88" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G5" s="63" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H5" s="63" t="s">
         <v>55</v>
       </c>
       <c r="I5" s="132" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="J5" s="197" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="K5" s="198"/>
       <c r="L5" s="198"/>
       <c r="M5" s="199"/>
       <c r="N5" s="126" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="O5" s="89" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="P5" s="76" t="s">
         <v>106</v>
       </c>
       <c r="Q5" s="75" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="R5" s="88" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="S5" s="64"/>
       <c r="T5" s="64"/>
@@ -10691,19 +11727,19 @@
       <c r="D6" s="33"/>
       <c r="E6" s="32"/>
       <c r="F6" s="88" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G6" s="63" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H6" s="63" t="s">
         <v>55</v>
       </c>
       <c r="I6" s="132" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="J6" s="197" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="K6" s="198"/>
       <c r="L6" s="198"/>
@@ -10712,16 +11748,16 @@
         <v>134</v>
       </c>
       <c r="O6" s="126" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="P6" s="76" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="Q6" s="75" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="R6" s="88" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="S6" s="64"/>
       <c r="T6" s="64"/>
@@ -10737,19 +11773,19 @@
       <c r="D7" s="33"/>
       <c r="E7" s="32"/>
       <c r="F7" s="88" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="G7" s="63" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H7" s="63" t="s">
         <v>55</v>
       </c>
       <c r="I7" s="132" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="J7" s="197" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="K7" s="198"/>
       <c r="L7" s="198"/>
@@ -10758,16 +11794,16 @@
         <v>134</v>
       </c>
       <c r="O7" s="126" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="P7" s="76" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="Q7" s="75" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="R7" s="82" t="s">
-        <v>216</v>
+        <v>228</v>
       </c>
       <c r="S7" s="64"/>
       <c r="T7" s="64"/>
@@ -10783,19 +11819,19 @@
       <c r="D8" s="33"/>
       <c r="E8" s="32"/>
       <c r="F8" s="88" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="G8" s="63" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H8" s="63" t="s">
         <v>55</v>
       </c>
       <c r="I8" s="132" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="J8" s="197" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="K8" s="198"/>
       <c r="L8" s="198"/>
@@ -10804,16 +11840,16 @@
         <v>134</v>
       </c>
       <c r="O8" s="126" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="P8" s="76" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="Q8" s="75" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="R8" s="82" t="s">
-        <v>217</v>
+        <v>229</v>
       </c>
       <c r="S8" s="64"/>
       <c r="T8" s="64"/>
@@ -10829,37 +11865,37 @@
       <c r="D9" s="33"/>
       <c r="E9" s="32"/>
       <c r="F9" s="88" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="G9" s="63" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H9" s="63" t="s">
         <v>55</v>
       </c>
       <c r="I9" s="132" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="J9" s="197" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="K9" s="198"/>
       <c r="L9" s="198"/>
       <c r="M9" s="199"/>
       <c r="N9" s="126" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="O9" s="126" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="P9" s="76" t="s">
-        <v>222</v>
+        <v>235</v>
       </c>
       <c r="Q9" s="75" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="R9" s="133" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="S9" s="64"/>
       <c r="T9" s="64"/>
@@ -12966,1114 +14002,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J87"/>
-  <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A13" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" customHeight="1"/>
-  <cols>
-    <col min="1" max="1" width="6.5703125" style="22" customWidth="1"/>
-    <col min="2" max="2" width="3.85546875" style="22" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" style="22" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" style="22" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" style="22" customWidth="1"/>
-    <col min="6" max="6" width="31.7109375" style="22" customWidth="1"/>
-    <col min="7" max="10" width="12.7109375" style="22" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="22"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" ht="12" customHeight="1">
-      <c r="A1" s="163" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="163"/>
-      <c r="C1" s="31" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="36" t="str">
-        <f>'Update History'!D1</f>
-        <v>ASOFT - ERP.NET</v>
-      </c>
-      <c r="E1" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="36" t="str">
-        <f>'Update History'!F1</f>
-        <v>CRMFXXX1</v>
-      </c>
-      <c r="G1" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="37" t="str">
-        <f>'Update History'!H1</f>
-        <v>Thị Phượng</v>
-      </c>
-      <c r="I1" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="67" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="12" customHeight="1">
-      <c r="A2" s="163"/>
-      <c r="B2" s="163"/>
-      <c r="C2" s="31" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="36" t="str">
-        <f>'Update History'!D2</f>
-        <v>ASOFT - CRM</v>
-      </c>
-      <c r="E2" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="36" t="str">
-        <f>'Update History'!F2</f>
-        <v>Báo cáo Khách hàng mới theo nhân viên</v>
-      </c>
-      <c r="G2" s="31" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="38">
-        <f>'Update History'!H2</f>
-        <v>42396</v>
-      </c>
-      <c r="I2" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="67">
-        <v>42396</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="12" customHeight="1">
-      <c r="A4" s="54"/>
-      <c r="B4" s="55"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="56"/>
-    </row>
-    <row r="5" spans="1:10" ht="12" customHeight="1">
-      <c r="A5" s="73" t="s">
-        <v>112</v>
-      </c>
-      <c r="B5" s="43"/>
-      <c r="C5" s="43"/>
-      <c r="D5" s="43"/>
-      <c r="E5" s="43"/>
-      <c r="F5" s="43"/>
-      <c r="G5" s="43"/>
-      <c r="H5" s="43"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="46"/>
-    </row>
-    <row r="6" spans="1:10" ht="12" customHeight="1">
-      <c r="A6" s="42"/>
-      <c r="B6" s="43"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="46"/>
-    </row>
-    <row r="7" spans="1:10" ht="12" customHeight="1">
-      <c r="A7" s="42"/>
-      <c r="B7" s="43"/>
-      <c r="C7" s="43"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="46"/>
-    </row>
-    <row r="8" spans="1:10" ht="12" customHeight="1">
-      <c r="A8" s="73" t="s">
-        <v>115</v>
-      </c>
-      <c r="B8" s="43"/>
-      <c r="C8" s="43"/>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="43"/>
-      <c r="I8" s="43"/>
-      <c r="J8" s="46"/>
-    </row>
-    <row r="9" spans="1:10" ht="12" customHeight="1">
-      <c r="A9" s="80"/>
-      <c r="B9" s="80" t="s">
-        <v>156</v>
-      </c>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
-      <c r="J9" s="46"/>
-    </row>
-    <row r="10" spans="1:10" ht="12" customHeight="1">
-      <c r="A10" s="80"/>
-      <c r="B10" s="43"/>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
-      <c r="I10" s="43"/>
-      <c r="J10" s="46"/>
-    </row>
-    <row r="11" spans="1:10" ht="12" customHeight="1">
-      <c r="A11" s="80"/>
-      <c r="B11" s="80" t="s">
-        <v>116</v>
-      </c>
-      <c r="C11" s="43"/>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
-      <c r="H11" s="43"/>
-      <c r="I11" s="43"/>
-      <c r="J11" s="46"/>
-    </row>
-    <row r="12" spans="1:10" ht="12" customHeight="1">
-      <c r="A12" s="80"/>
-      <c r="B12" s="43"/>
-      <c r="C12" s="43"/>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="43"/>
-      <c r="I12" s="43"/>
-      <c r="J12" s="46"/>
-    </row>
-    <row r="13" spans="1:10" ht="12" customHeight="1">
-      <c r="A13" s="80"/>
-      <c r="B13" s="43"/>
-      <c r="C13" s="43"/>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="43"/>
-      <c r="I13" s="43"/>
-      <c r="J13" s="46"/>
-    </row>
-    <row r="14" spans="1:10" ht="12" customHeight="1">
-      <c r="B14" s="80" t="s">
-        <v>117</v>
-      </c>
-      <c r="C14" s="43"/>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="43"/>
-      <c r="I14" s="43"/>
-      <c r="J14" s="46"/>
-    </row>
-    <row r="16" spans="1:10" ht="12" customHeight="1">
-      <c r="B16" s="80" t="s">
-        <v>118</v>
-      </c>
-      <c r="C16" s="43"/>
-      <c r="D16" s="43"/>
-      <c r="E16" s="43"/>
-      <c r="F16" s="43"/>
-      <c r="G16" s="43"/>
-      <c r="H16" s="43"/>
-      <c r="I16" s="43"/>
-      <c r="J16" s="46"/>
-    </row>
-    <row r="17" spans="1:10" ht="12" customHeight="1">
-      <c r="B17" s="43"/>
-      <c r="C17" s="43" t="s">
-        <v>218</v>
-      </c>
-      <c r="D17" s="43"/>
-      <c r="E17" s="43"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="43"/>
-      <c r="H17" s="43"/>
-      <c r="I17" s="43"/>
-      <c r="J17" s="46"/>
-    </row>
-    <row r="18" spans="1:10" ht="12" customHeight="1">
-      <c r="B18" s="43"/>
-      <c r="C18" s="43"/>
-      <c r="D18" s="43"/>
-      <c r="E18" s="43"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="43"/>
-      <c r="H18" s="43"/>
-      <c r="I18" s="43"/>
-      <c r="J18" s="46"/>
-    </row>
-    <row r="19" spans="1:10" ht="12" customHeight="1">
-      <c r="B19" s="80" t="s">
-        <v>119</v>
-      </c>
-      <c r="C19" s="43"/>
-      <c r="D19" s="43"/>
-      <c r="E19" s="43"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="43"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="43"/>
-      <c r="J19" s="46"/>
-    </row>
-    <row r="20" spans="1:10" ht="12" customHeight="1">
-      <c r="B20" s="43"/>
-      <c r="D20" s="43"/>
-      <c r="E20" s="43"/>
-      <c r="F20" s="43"/>
-      <c r="G20" s="43"/>
-      <c r="H20" s="43"/>
-      <c r="I20" s="43"/>
-      <c r="J20" s="46"/>
-    </row>
-    <row r="21" spans="1:10" ht="12" customHeight="1">
-      <c r="B21" s="43"/>
-      <c r="C21" s="43"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="43"/>
-      <c r="G21" s="43"/>
-      <c r="H21" s="43"/>
-      <c r="I21" s="43"/>
-      <c r="J21" s="46"/>
-    </row>
-    <row r="22" spans="1:10" ht="12" customHeight="1">
-      <c r="B22" s="80" t="s">
-        <v>120</v>
-      </c>
-      <c r="C22" s="43"/>
-      <c r="D22" s="43"/>
-      <c r="E22" s="43"/>
-      <c r="F22" s="43"/>
-      <c r="G22" s="43"/>
-      <c r="H22" s="43"/>
-      <c r="I22" s="43"/>
-      <c r="J22" s="46"/>
-    </row>
-    <row r="23" spans="1:10" ht="12" customHeight="1">
-      <c r="B23" s="80"/>
-      <c r="C23" s="43"/>
-      <c r="D23" s="43"/>
-      <c r="E23" s="43"/>
-      <c r="F23" s="43"/>
-      <c r="G23" s="43"/>
-      <c r="H23" s="43"/>
-      <c r="I23" s="43"/>
-      <c r="J23" s="46"/>
-    </row>
-    <row r="24" spans="1:10" ht="12" customHeight="1">
-      <c r="A24" s="42"/>
-      <c r="B24" s="43"/>
-      <c r="C24" s="43"/>
-      <c r="D24" s="43"/>
-      <c r="E24" s="43"/>
-      <c r="F24" s="43"/>
-      <c r="G24" s="43"/>
-      <c r="H24" s="43"/>
-      <c r="I24" s="43"/>
-      <c r="J24" s="46"/>
-    </row>
-    <row r="25" spans="1:10" ht="12" customHeight="1">
-      <c r="A25" s="73" t="s">
-        <v>114</v>
-      </c>
-      <c r="B25" s="43"/>
-      <c r="C25" s="43"/>
-      <c r="D25" s="43"/>
-      <c r="E25" s="43"/>
-      <c r="F25" s="43"/>
-      <c r="G25" s="43"/>
-      <c r="H25" s="43"/>
-      <c r="I25" s="43"/>
-      <c r="J25" s="46"/>
-    </row>
-    <row r="26" spans="1:10" ht="12" customHeight="1">
-      <c r="A26" s="73"/>
-      <c r="B26" s="43" t="s">
-        <v>219</v>
-      </c>
-      <c r="C26" s="43"/>
-      <c r="D26" s="43"/>
-      <c r="E26" s="43"/>
-      <c r="F26" s="43"/>
-      <c r="G26" s="43"/>
-      <c r="H26" s="43"/>
-      <c r="I26" s="43"/>
-      <c r="J26" s="46"/>
-    </row>
-    <row r="27" spans="1:10" ht="12" customHeight="1">
-      <c r="A27" s="42"/>
-      <c r="B27" s="86"/>
-      <c r="C27" s="86"/>
-      <c r="D27" s="43"/>
-      <c r="E27" s="43"/>
-      <c r="F27" s="43"/>
-      <c r="G27" s="43"/>
-      <c r="H27" s="43"/>
-      <c r="I27" s="43"/>
-      <c r="J27" s="46"/>
-    </row>
-    <row r="28" spans="1:10" ht="12" customHeight="1">
-      <c r="A28" s="73" t="s">
-        <v>123</v>
-      </c>
-      <c r="B28" s="43"/>
-      <c r="C28" s="86"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="43"/>
-      <c r="I28" s="43"/>
-      <c r="J28" s="46"/>
-    </row>
-    <row r="29" spans="1:10" ht="12" customHeight="1">
-      <c r="B29" s="80" t="s">
-        <v>121</v>
-      </c>
-      <c r="C29" s="86"/>
-      <c r="D29" s="43"/>
-      <c r="E29" s="43"/>
-      <c r="F29" s="43"/>
-      <c r="G29" s="43"/>
-      <c r="H29" s="43"/>
-      <c r="I29" s="43"/>
-      <c r="J29" s="46"/>
-    </row>
-    <row r="30" spans="1:10" ht="12" customHeight="1">
-      <c r="B30" s="43"/>
-      <c r="C30" s="86"/>
-      <c r="D30" s="43"/>
-      <c r="E30" s="43"/>
-      <c r="F30" s="43"/>
-      <c r="G30" s="43"/>
-      <c r="H30" s="43"/>
-      <c r="I30" s="43"/>
-      <c r="J30" s="46"/>
-    </row>
-    <row r="31" spans="1:10" ht="12" customHeight="1">
-      <c r="B31" s="43"/>
-      <c r="C31" s="86"/>
-      <c r="D31" s="43"/>
-      <c r="E31" s="43"/>
-      <c r="F31" s="43"/>
-      <c r="G31" s="43"/>
-      <c r="H31" s="43"/>
-      <c r="I31" s="43"/>
-      <c r="J31" s="46"/>
-    </row>
-    <row r="32" spans="1:10" ht="12" customHeight="1">
-      <c r="B32" s="80" t="s">
-        <v>122</v>
-      </c>
-      <c r="C32" s="43"/>
-      <c r="D32" s="43"/>
-      <c r="E32" s="43"/>
-      <c r="F32" s="43"/>
-      <c r="G32" s="43"/>
-      <c r="H32" s="43"/>
-      <c r="I32" s="43"/>
-      <c r="J32" s="46"/>
-    </row>
-    <row r="33" spans="1:10" ht="12" customHeight="1">
-      <c r="B33" s="80"/>
-      <c r="C33" s="86"/>
-      <c r="D33" s="43"/>
-      <c r="E33" s="43"/>
-      <c r="F33" s="43"/>
-      <c r="G33" s="43"/>
-      <c r="H33" s="43"/>
-      <c r="I33" s="43"/>
-      <c r="J33" s="46"/>
-    </row>
-    <row r="34" spans="1:10" ht="12" customHeight="1">
-      <c r="A34" s="42"/>
-      <c r="B34" s="43"/>
-      <c r="C34" s="43"/>
-      <c r="D34" s="43"/>
-      <c r="E34" s="43"/>
-      <c r="F34" s="43"/>
-      <c r="G34" s="43"/>
-      <c r="H34" s="43"/>
-      <c r="I34" s="43"/>
-      <c r="J34" s="46"/>
-    </row>
-    <row r="35" spans="1:10" ht="12" customHeight="1">
-      <c r="A35" s="73" t="s">
-        <v>124</v>
-      </c>
-      <c r="B35" s="43"/>
-      <c r="C35" s="86"/>
-      <c r="D35" s="43"/>
-      <c r="E35" s="43"/>
-      <c r="F35" s="43"/>
-      <c r="G35" s="43"/>
-      <c r="H35" s="43"/>
-      <c r="I35" s="43"/>
-      <c r="J35" s="46"/>
-    </row>
-    <row r="36" spans="1:10" ht="12" customHeight="1">
-      <c r="B36" s="80" t="s">
-        <v>121</v>
-      </c>
-      <c r="C36" s="86"/>
-      <c r="D36" s="43"/>
-      <c r="E36" s="43"/>
-      <c r="F36" s="43"/>
-      <c r="G36" s="43"/>
-      <c r="H36" s="43"/>
-      <c r="I36" s="43"/>
-      <c r="J36" s="46"/>
-    </row>
-    <row r="37" spans="1:10" ht="12" customHeight="1">
-      <c r="B37" s="43"/>
-      <c r="C37" s="86"/>
-      <c r="D37" s="43"/>
-      <c r="E37" s="43"/>
-      <c r="F37" s="43"/>
-      <c r="G37" s="43"/>
-      <c r="H37" s="43"/>
-      <c r="I37" s="43"/>
-      <c r="J37" s="46"/>
-    </row>
-    <row r="38" spans="1:10" ht="12" customHeight="1">
-      <c r="B38" s="43"/>
-      <c r="C38" s="86"/>
-      <c r="D38" s="43"/>
-      <c r="E38" s="43"/>
-      <c r="F38" s="43"/>
-      <c r="G38" s="43"/>
-      <c r="H38" s="43"/>
-      <c r="I38" s="43"/>
-      <c r="J38" s="46"/>
-    </row>
-    <row r="39" spans="1:10" ht="12" customHeight="1">
-      <c r="B39" s="80" t="s">
-        <v>122</v>
-      </c>
-      <c r="C39" s="43"/>
-      <c r="D39" s="43"/>
-      <c r="E39" s="43"/>
-      <c r="F39" s="43"/>
-      <c r="G39" s="43"/>
-      <c r="H39" s="43"/>
-      <c r="I39" s="43"/>
-      <c r="J39" s="46"/>
-    </row>
-    <row r="40" spans="1:10" ht="12" customHeight="1">
-      <c r="B40" s="80"/>
-      <c r="C40" s="86"/>
-      <c r="D40" s="43"/>
-      <c r="E40" s="43"/>
-      <c r="F40" s="43"/>
-      <c r="G40" s="43"/>
-      <c r="H40" s="43"/>
-      <c r="I40" s="43"/>
-      <c r="J40" s="46"/>
-    </row>
-    <row r="41" spans="1:10" ht="12" customHeight="1">
-      <c r="A41" s="42"/>
-      <c r="B41" s="86"/>
-      <c r="C41" s="43"/>
-      <c r="D41" s="43"/>
-      <c r="E41" s="43"/>
-      <c r="F41" s="43"/>
-      <c r="G41" s="43"/>
-      <c r="H41" s="43"/>
-      <c r="I41" s="43"/>
-      <c r="J41" s="46"/>
-    </row>
-    <row r="42" spans="1:10" ht="12" customHeight="1">
-      <c r="A42" s="73" t="s">
-        <v>125</v>
-      </c>
-      <c r="B42" s="43"/>
-      <c r="C42" s="86"/>
-      <c r="D42" s="43"/>
-      <c r="E42" s="43"/>
-      <c r="F42" s="43"/>
-      <c r="G42" s="43"/>
-      <c r="H42" s="43"/>
-      <c r="I42" s="43"/>
-      <c r="J42" s="46"/>
-    </row>
-    <row r="43" spans="1:10" ht="12" customHeight="1">
-      <c r="B43" s="80" t="s">
-        <v>126</v>
-      </c>
-      <c r="C43" s="86"/>
-      <c r="D43" s="43"/>
-      <c r="E43" s="43"/>
-      <c r="F43" s="43"/>
-      <c r="G43" s="43"/>
-      <c r="H43" s="43"/>
-      <c r="I43" s="43"/>
-      <c r="J43" s="46"/>
-    </row>
-    <row r="44" spans="1:10" ht="12" customHeight="1">
-      <c r="B44" s="80"/>
-      <c r="C44" s="86"/>
-      <c r="D44" s="43"/>
-      <c r="E44" s="43"/>
-      <c r="F44" s="43"/>
-      <c r="G44" s="43"/>
-      <c r="H44" s="43"/>
-      <c r="I44" s="43"/>
-      <c r="J44" s="46"/>
-    </row>
-    <row r="45" spans="1:10" ht="12" customHeight="1">
-      <c r="B45" s="43"/>
-      <c r="C45" s="86"/>
-      <c r="D45" s="43"/>
-      <c r="E45" s="43"/>
-      <c r="F45" s="43"/>
-      <c r="G45" s="43"/>
-      <c r="H45" s="43"/>
-      <c r="I45" s="43"/>
-      <c r="J45" s="46"/>
-    </row>
-    <row r="46" spans="1:10" ht="12" customHeight="1">
-      <c r="B46" s="80" t="s">
-        <v>127</v>
-      </c>
-      <c r="C46" s="43"/>
-      <c r="D46" s="43"/>
-      <c r="E46" s="43"/>
-      <c r="F46" s="43"/>
-      <c r="G46" s="43"/>
-      <c r="H46" s="43"/>
-      <c r="I46" s="43"/>
-      <c r="J46" s="46"/>
-    </row>
-    <row r="47" spans="1:10" ht="12" customHeight="1">
-      <c r="B47" s="80"/>
-      <c r="C47" s="43"/>
-      <c r="D47" s="43"/>
-      <c r="E47" s="43"/>
-      <c r="F47" s="43"/>
-      <c r="G47" s="43"/>
-      <c r="H47" s="43"/>
-      <c r="I47" s="43"/>
-      <c r="J47" s="46"/>
-    </row>
-    <row r="48" spans="1:10" ht="12" customHeight="1">
-      <c r="A48" s="73" t="s">
-        <v>128</v>
-      </c>
-      <c r="B48" s="43"/>
-      <c r="C48" s="86"/>
-      <c r="D48" s="43"/>
-      <c r="E48" s="43"/>
-      <c r="F48" s="43"/>
-      <c r="G48" s="43"/>
-      <c r="H48" s="43"/>
-      <c r="I48" s="43"/>
-      <c r="J48" s="46"/>
-    </row>
-    <row r="49" spans="1:10" ht="12" customHeight="1">
-      <c r="B49" s="80" t="s">
-        <v>199</v>
-      </c>
-      <c r="C49" s="86"/>
-      <c r="D49" s="43"/>
-      <c r="E49" s="43"/>
-      <c r="F49" s="43"/>
-      <c r="G49" s="43"/>
-      <c r="H49" s="43"/>
-      <c r="I49" s="43"/>
-      <c r="J49" s="46"/>
-    </row>
-    <row r="50" spans="1:10" ht="12" customHeight="1">
-      <c r="B50" s="43"/>
-      <c r="C50" s="86"/>
-      <c r="D50" s="43"/>
-      <c r="E50" s="43"/>
-      <c r="F50" s="43"/>
-      <c r="G50" s="43"/>
-      <c r="H50" s="43"/>
-      <c r="I50" s="43"/>
-      <c r="J50" s="46"/>
-    </row>
-    <row r="51" spans="1:10" ht="12" customHeight="1">
-      <c r="B51" s="80"/>
-      <c r="C51" s="43"/>
-      <c r="D51" s="43"/>
-      <c r="E51" s="43"/>
-      <c r="F51" s="43"/>
-      <c r="G51" s="43"/>
-      <c r="H51" s="43"/>
-      <c r="I51" s="43"/>
-      <c r="J51" s="46"/>
-    </row>
-    <row r="52" spans="1:10" ht="12" customHeight="1">
-      <c r="B52" s="80"/>
-      <c r="C52" s="43"/>
-      <c r="D52" s="43"/>
-      <c r="E52" s="43"/>
-      <c r="F52" s="43"/>
-      <c r="G52" s="43"/>
-      <c r="H52" s="43"/>
-      <c r="I52" s="43"/>
-      <c r="J52" s="46"/>
-    </row>
-    <row r="53" spans="1:10" ht="12" customHeight="1">
-      <c r="B53" s="43"/>
-      <c r="C53" s="43"/>
-      <c r="D53" s="43"/>
-      <c r="E53" s="43"/>
-      <c r="F53" s="43"/>
-      <c r="G53" s="43"/>
-      <c r="H53" s="43"/>
-      <c r="I53" s="43"/>
-      <c r="J53" s="46"/>
-    </row>
-    <row r="54" spans="1:10" ht="12" customHeight="1">
-      <c r="B54" s="43"/>
-      <c r="C54" s="43"/>
-      <c r="D54" s="43"/>
-      <c r="E54" s="43"/>
-      <c r="F54" s="43"/>
-      <c r="G54" s="43"/>
-      <c r="H54" s="43"/>
-      <c r="I54" s="43"/>
-      <c r="J54" s="46"/>
-    </row>
-    <row r="55" spans="1:10" ht="12" customHeight="1">
-      <c r="B55" s="80"/>
-      <c r="C55" s="43"/>
-      <c r="D55" s="43"/>
-      <c r="E55" s="43"/>
-      <c r="F55" s="43"/>
-      <c r="G55" s="43"/>
-      <c r="H55" s="43"/>
-      <c r="I55" s="43"/>
-      <c r="J55" s="46"/>
-    </row>
-    <row r="56" spans="1:10" ht="12" customHeight="1">
-      <c r="A56" s="42"/>
-      <c r="B56" s="43"/>
-      <c r="C56" s="86"/>
-      <c r="D56" s="43"/>
-      <c r="E56" s="43"/>
-      <c r="F56" s="43"/>
-      <c r="G56" s="43"/>
-      <c r="H56" s="43"/>
-      <c r="I56" s="43"/>
-      <c r="J56" s="46"/>
-    </row>
-    <row r="57" spans="1:10" ht="12" customHeight="1">
-      <c r="A57" s="42"/>
-      <c r="B57" s="43"/>
-      <c r="C57" s="86"/>
-      <c r="D57" s="43"/>
-      <c r="E57" s="43"/>
-      <c r="F57" s="43"/>
-      <c r="G57" s="43"/>
-      <c r="H57" s="43"/>
-      <c r="I57" s="43"/>
-      <c r="J57" s="46"/>
-    </row>
-    <row r="58" spans="1:10" ht="12" customHeight="1">
-      <c r="A58" s="42"/>
-      <c r="B58" s="43"/>
-      <c r="C58" s="86"/>
-      <c r="D58" s="43"/>
-      <c r="E58" s="43"/>
-      <c r="F58" s="43"/>
-      <c r="G58" s="43"/>
-      <c r="H58" s="43"/>
-      <c r="I58" s="43"/>
-      <c r="J58" s="46"/>
-    </row>
-    <row r="59" spans="1:10" ht="12" customHeight="1">
-      <c r="A59" s="73"/>
-      <c r="B59" s="43"/>
-      <c r="C59" s="43"/>
-      <c r="D59" s="43"/>
-      <c r="E59" s="43"/>
-      <c r="F59" s="43"/>
-      <c r="G59" s="43"/>
-      <c r="H59" s="43"/>
-      <c r="I59" s="43"/>
-      <c r="J59" s="46"/>
-    </row>
-    <row r="60" spans="1:10" ht="12" customHeight="1">
-      <c r="B60" s="80"/>
-      <c r="C60" s="43"/>
-      <c r="D60" s="43"/>
-      <c r="E60" s="43"/>
-      <c r="F60" s="43"/>
-      <c r="G60" s="43"/>
-      <c r="H60" s="43"/>
-      <c r="I60" s="43"/>
-      <c r="J60" s="46"/>
-    </row>
-    <row r="61" spans="1:10" ht="12" customHeight="1">
-      <c r="B61" s="43"/>
-      <c r="C61" s="43"/>
-      <c r="D61" s="43"/>
-      <c r="E61" s="43"/>
-      <c r="F61" s="43"/>
-      <c r="G61" s="43"/>
-      <c r="H61" s="43"/>
-      <c r="I61" s="43"/>
-      <c r="J61" s="46"/>
-    </row>
-    <row r="62" spans="1:10" ht="12" customHeight="1">
-      <c r="B62" s="80"/>
-      <c r="C62" s="43"/>
-      <c r="D62" s="43"/>
-      <c r="E62" s="43"/>
-      <c r="F62" s="43"/>
-      <c r="G62" s="43"/>
-      <c r="H62" s="43"/>
-      <c r="I62" s="43"/>
-      <c r="J62" s="46"/>
-    </row>
-    <row r="63" spans="1:10" ht="12" customHeight="1">
-      <c r="A63" s="42"/>
-      <c r="B63" s="43"/>
-      <c r="C63" s="43"/>
-      <c r="D63" s="43"/>
-      <c r="E63" s="43"/>
-      <c r="F63" s="43"/>
-      <c r="G63" s="43"/>
-      <c r="H63" s="43"/>
-      <c r="I63" s="43"/>
-      <c r="J63" s="46"/>
-    </row>
-    <row r="64" spans="1:10" ht="12" customHeight="1">
-      <c r="A64" s="73"/>
-      <c r="B64" s="43"/>
-      <c r="C64" s="43"/>
-      <c r="D64" s="43"/>
-      <c r="E64" s="43"/>
-      <c r="F64" s="43"/>
-      <c r="G64" s="43"/>
-      <c r="H64" s="43"/>
-      <c r="I64" s="43"/>
-      <c r="J64" s="46"/>
-    </row>
-    <row r="65" spans="1:10" ht="12" customHeight="1">
-      <c r="A65" s="42"/>
-      <c r="B65" s="43"/>
-      <c r="C65" s="43"/>
-      <c r="D65" s="43"/>
-      <c r="E65" s="43"/>
-      <c r="F65" s="43"/>
-      <c r="G65" s="43"/>
-      <c r="H65" s="43"/>
-      <c r="I65" s="43"/>
-      <c r="J65" s="46"/>
-    </row>
-    <row r="66" spans="1:10" ht="12" customHeight="1">
-      <c r="A66" s="42"/>
-      <c r="B66" s="43"/>
-      <c r="C66" s="43"/>
-      <c r="D66" s="43"/>
-      <c r="E66" s="43"/>
-      <c r="F66" s="43"/>
-      <c r="G66" s="43"/>
-      <c r="H66" s="43"/>
-      <c r="I66" s="43"/>
-      <c r="J66" s="46"/>
-    </row>
-    <row r="67" spans="1:10" ht="12" customHeight="1">
-      <c r="A67" s="42"/>
-      <c r="B67" s="43"/>
-      <c r="C67" s="43"/>
-      <c r="D67" s="43"/>
-      <c r="E67" s="43"/>
-      <c r="F67" s="43"/>
-      <c r="G67" s="43"/>
-      <c r="H67" s="43"/>
-      <c r="I67" s="43"/>
-      <c r="J67" s="46"/>
-    </row>
-    <row r="68" spans="1:10" ht="12" customHeight="1">
-      <c r="A68" s="42"/>
-      <c r="B68" s="43"/>
-      <c r="C68" s="43"/>
-      <c r="D68" s="43"/>
-      <c r="E68" s="43"/>
-      <c r="F68" s="43"/>
-      <c r="G68" s="43"/>
-      <c r="H68" s="43"/>
-      <c r="I68" s="43"/>
-      <c r="J68" s="46"/>
-    </row>
-    <row r="69" spans="1:10" ht="12" customHeight="1">
-      <c r="A69" s="42"/>
-      <c r="B69" s="43"/>
-      <c r="C69" s="43"/>
-      <c r="D69" s="43"/>
-      <c r="E69" s="43"/>
-      <c r="F69" s="43"/>
-      <c r="G69" s="43"/>
-      <c r="H69" s="43"/>
-      <c r="I69" s="43"/>
-      <c r="J69" s="46"/>
-    </row>
-    <row r="70" spans="1:10" ht="12" customHeight="1">
-      <c r="A70" s="42"/>
-      <c r="B70" s="43"/>
-      <c r="C70" s="43"/>
-      <c r="D70" s="43"/>
-      <c r="E70" s="43"/>
-      <c r="F70" s="43"/>
-      <c r="G70" s="43"/>
-      <c r="H70" s="43"/>
-      <c r="I70" s="43"/>
-      <c r="J70" s="46"/>
-    </row>
-    <row r="71" spans="1:10" ht="12" customHeight="1">
-      <c r="A71" s="42"/>
-      <c r="B71" s="43"/>
-      <c r="C71" s="43"/>
-      <c r="D71" s="43"/>
-      <c r="E71" s="43"/>
-      <c r="F71" s="43"/>
-      <c r="G71" s="43"/>
-      <c r="H71" s="43"/>
-      <c r="I71" s="43"/>
-      <c r="J71" s="46"/>
-    </row>
-    <row r="72" spans="1:10" ht="12" customHeight="1">
-      <c r="A72" s="42"/>
-      <c r="B72" s="43"/>
-      <c r="C72" s="43"/>
-      <c r="D72" s="43"/>
-      <c r="E72" s="43"/>
-      <c r="F72" s="43"/>
-      <c r="G72" s="43"/>
-      <c r="H72" s="43"/>
-      <c r="I72" s="43"/>
-      <c r="J72" s="46"/>
-    </row>
-    <row r="73" spans="1:10" ht="12" customHeight="1">
-      <c r="A73" s="42"/>
-      <c r="B73" s="43"/>
-      <c r="C73" s="43"/>
-      <c r="D73" s="43"/>
-      <c r="E73" s="43"/>
-      <c r="F73" s="43"/>
-      <c r="G73" s="43"/>
-      <c r="H73" s="43"/>
-      <c r="I73" s="43"/>
-      <c r="J73" s="46"/>
-    </row>
-    <row r="74" spans="1:10" ht="12" customHeight="1">
-      <c r="A74" s="42"/>
-      <c r="B74" s="43"/>
-      <c r="C74" s="43"/>
-      <c r="D74" s="43"/>
-      <c r="E74" s="43"/>
-      <c r="F74" s="43"/>
-      <c r="G74" s="43"/>
-      <c r="H74" s="43"/>
-      <c r="I74" s="43"/>
-      <c r="J74" s="46"/>
-    </row>
-    <row r="75" spans="1:10" ht="12" customHeight="1">
-      <c r="A75" s="42"/>
-      <c r="B75" s="43"/>
-      <c r="C75" s="43"/>
-      <c r="D75" s="43"/>
-      <c r="E75" s="43"/>
-      <c r="F75" s="43"/>
-      <c r="G75" s="43"/>
-      <c r="H75" s="43"/>
-      <c r="I75" s="43"/>
-      <c r="J75" s="46"/>
-    </row>
-    <row r="76" spans="1:10" ht="12" customHeight="1">
-      <c r="A76" s="42"/>
-      <c r="B76" s="43"/>
-      <c r="C76" s="43"/>
-      <c r="D76" s="43"/>
-      <c r="E76" s="43"/>
-      <c r="F76" s="43"/>
-      <c r="G76" s="43"/>
-      <c r="H76" s="43"/>
-      <c r="I76" s="43"/>
-      <c r="J76" s="46"/>
-    </row>
-    <row r="77" spans="1:10" ht="12" customHeight="1">
-      <c r="A77" s="42"/>
-      <c r="B77" s="43"/>
-      <c r="C77" s="43"/>
-      <c r="D77" s="43"/>
-      <c r="E77" s="43"/>
-      <c r="F77" s="43"/>
-      <c r="G77" s="43"/>
-      <c r="H77" s="43"/>
-      <c r="I77" s="43"/>
-      <c r="J77" s="46"/>
-    </row>
-    <row r="78" spans="1:10" ht="12" customHeight="1">
-      <c r="A78" s="42"/>
-      <c r="B78" s="43"/>
-      <c r="C78" s="43"/>
-      <c r="D78" s="43"/>
-      <c r="E78" s="43"/>
-      <c r="F78" s="43"/>
-      <c r="G78" s="43"/>
-      <c r="H78" s="43"/>
-      <c r="I78" s="43"/>
-      <c r="J78" s="46"/>
-    </row>
-    <row r="79" spans="1:10" ht="12" customHeight="1">
-      <c r="A79" s="42"/>
-      <c r="B79" s="43"/>
-      <c r="C79" s="43"/>
-      <c r="D79" s="43"/>
-      <c r="E79" s="43"/>
-      <c r="F79" s="43"/>
-      <c r="G79" s="43"/>
-      <c r="H79" s="43"/>
-      <c r="I79" s="43"/>
-      <c r="J79" s="46"/>
-    </row>
-    <row r="80" spans="1:10" ht="12" customHeight="1">
-      <c r="A80" s="42"/>
-      <c r="B80" s="43"/>
-      <c r="C80" s="43"/>
-      <c r="D80" s="43"/>
-      <c r="E80" s="43"/>
-      <c r="F80" s="43"/>
-      <c r="G80" s="43"/>
-      <c r="H80" s="43"/>
-      <c r="I80" s="43"/>
-      <c r="J80" s="46"/>
-    </row>
-    <row r="81" spans="1:10" ht="12" customHeight="1">
-      <c r="A81" s="42"/>
-      <c r="B81" s="43"/>
-      <c r="C81" s="43"/>
-      <c r="D81" s="43"/>
-      <c r="E81" s="43"/>
-      <c r="F81" s="43"/>
-      <c r="G81" s="43"/>
-      <c r="H81" s="43"/>
-      <c r="I81" s="43"/>
-      <c r="J81" s="46"/>
-    </row>
-    <row r="82" spans="1:10" ht="12" customHeight="1">
-      <c r="A82" s="42"/>
-      <c r="B82" s="43"/>
-      <c r="C82" s="43"/>
-      <c r="D82" s="43"/>
-      <c r="E82" s="43"/>
-      <c r="F82" s="43"/>
-      <c r="G82" s="43"/>
-      <c r="H82" s="43"/>
-      <c r="I82" s="43"/>
-      <c r="J82" s="46"/>
-    </row>
-    <row r="83" spans="1:10" ht="12" customHeight="1">
-      <c r="A83" s="42"/>
-      <c r="B83" s="43"/>
-      <c r="C83" s="43"/>
-      <c r="D83" s="43"/>
-      <c r="E83" s="43"/>
-      <c r="F83" s="43"/>
-      <c r="G83" s="43"/>
-      <c r="H83" s="43"/>
-      <c r="I83" s="43"/>
-      <c r="J83" s="46"/>
-    </row>
-    <row r="84" spans="1:10" ht="12" customHeight="1">
-      <c r="A84" s="42"/>
-      <c r="B84" s="43"/>
-      <c r="C84" s="43"/>
-      <c r="D84" s="43"/>
-      <c r="E84" s="43"/>
-      <c r="F84" s="43"/>
-      <c r="G84" s="43"/>
-      <c r="H84" s="43"/>
-      <c r="I84" s="43"/>
-      <c r="J84" s="46"/>
-    </row>
-    <row r="85" spans="1:10" ht="12" customHeight="1">
-      <c r="A85" s="42"/>
-      <c r="B85" s="43"/>
-      <c r="C85" s="43"/>
-      <c r="D85" s="43"/>
-      <c r="E85" s="43"/>
-      <c r="F85" s="43"/>
-      <c r="G85" s="43"/>
-      <c r="H85" s="43"/>
-      <c r="I85" s="43"/>
-      <c r="J85" s="46"/>
-    </row>
-    <row r="86" spans="1:10" ht="12" customHeight="1">
-      <c r="A86" s="42"/>
-      <c r="B86" s="43"/>
-      <c r="C86" s="43"/>
-      <c r="D86" s="43"/>
-      <c r="E86" s="43"/>
-      <c r="F86" s="43"/>
-      <c r="G86" s="43"/>
-      <c r="H86" s="43"/>
-      <c r="I86" s="43"/>
-      <c r="J86" s="46"/>
-    </row>
-    <row r="87" spans="1:10" ht="12" customHeight="1">
-      <c r="A87" s="47"/>
-      <c r="B87" s="48"/>
-      <c r="C87" s="48"/>
-      <c r="D87" s="48"/>
-      <c r="E87" s="48"/>
-      <c r="F87" s="48"/>
-      <c r="G87" s="48"/>
-      <c r="H87" s="48"/>
-      <c r="I87" s="48"/>
-      <c r="J87" s="57"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:B2"/>
-  </mergeCells>
-  <pageMargins left="0.3" right="0.3" top="0.6" bottom="0.3" header="0.1" footer="0.1"/>
-  <pageSetup paperSize="9" scale="81" orientation="landscape" r:id="rId1"/>
-  <headerFooter>
-    <oddHeader>&amp;R&amp;G</oddHeader>
-    <oddFooter>&amp;L&amp;"Ta,Regular"&amp;10CONFIDENTIAL&amp;C&amp;"Tahoma,Regular"&amp;10&amp;P&amp;R&amp;"Tahoma,Regular"&amp;10© 2010 ASOFT JSC. All rights reserved.</oddFooter>
-  </headerFooter>
-  <rowBreaks count="2" manualBreakCount="2">
-    <brk id="52" max="9" man="1"/>
-    <brk id="65" max="9" man="1"/>
-  </rowBreaks>
-  <legacyDrawing r:id="rId2"/>
-  <legacyDrawingHF r:id="rId3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J32"/>
@@ -14111,7 +14039,7 @@
       </c>
       <c r="F1" s="36" t="str">
         <f>'Update History'!F1</f>
-        <v>CRMFXXX1</v>
+        <v>CRMF3010</v>
       </c>
       <c r="G1" s="31" t="s">
         <v>5</v>

</xml_diff>